<commit_message>
Better sorting and ordering.
</commit_message>
<xml_diff>
--- a/TestSheet.xlsx
+++ b/TestSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_09CE59F3B32C71B27447F41703FFAE311A56176B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6041915-5DE2-4423-8318-86994A3A4619}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_09CE59F3B32C71B27447F41703FFAE311A56176B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25E90753-C37E-40A0-BE4D-959040AE3F19}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -415,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H107" authorId="0" shapeId="0" xr:uid="{2BC63E99-34BF-4D42-8655-E335DD0592F9}">
+    <comment ref="H107" authorId="0" shapeId="0" xr:uid="{77F56855-BB6A-4B5F-B133-6297B728430C}">
       <text>
         <r>
           <rPr>
@@ -429,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B149" authorId="0" shapeId="0" xr:uid="{3D34FEBE-0C30-40A8-A0CB-B77FE8452FE8}">
+    <comment ref="B151" authorId="0" shapeId="0" xr:uid="{3D34FEBE-0C30-40A8-A0CB-B77FE8452FE8}">
       <text>
         <r>
           <rPr>
@@ -442,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B150" authorId="0" shapeId="0" xr:uid="{E69FFF4D-4063-4C08-868F-30EB9D45B452}">
+    <comment ref="B152" authorId="0" shapeId="0" xr:uid="{E69FFF4D-4063-4C08-868F-30EB9D45B452}">
       <text>
         <r>
           <rPr>
@@ -455,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B151" authorId="0" shapeId="0" xr:uid="{3D1198C2-7F58-4A8C-B5C4-D37AAD6330CC}">
+    <comment ref="B153" authorId="0" shapeId="0" xr:uid="{3D1198C2-7F58-4A8C-B5C4-D37AAD6330CC}">
       <text>
         <r>
           <rPr>
@@ -473,7 +473,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3587" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3597" uniqueCount="189">
   <si>
     <t>Code</t>
   </si>
@@ -1049,12 +1049,21 @@
   <si>
     <t>Hello World</t>
   </si>
+  <si>
+    <t>Boss</t>
+  </si>
+  <si>
+    <t>X01</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1225,8 +1234,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Amasis MT Pro"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Amasis MT Pro"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1329,6 +1359,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -1420,7 +1480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1576,12 +1636,33 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="25" fillId="21" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99FF99"/>
+      <color rgb="FF66FF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -18025,11 +18106,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1155"/>
+  <dimension ref="A1:Z1157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19872,7 +19953,7 @@
       <c r="Z42" s="27"/>
     </row>
     <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="32" t="s">
+      <c r="A43" s="25" t="s">
         <v>58</v>
       </c>
       <c r="B43" s="26" t="s">
@@ -20788,7 +20869,7 @@
       <c r="Z63" s="27"/>
     </row>
     <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="42" t="s">
+      <c r="A64" s="41" t="s">
         <v>81</v>
       </c>
       <c r="B64" s="26" t="s">
@@ -21704,7 +21785,7 @@
       <c r="Z84" s="27"/>
     </row>
     <row r="85" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="42" t="s">
+      <c r="A85" s="41" t="s">
         <v>104</v>
       </c>
       <c r="B85" s="26" t="s">
@@ -22620,7 +22701,7 @@
       <c r="Z105" s="27"/>
     </row>
     <row r="106" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="42" t="s">
+      <c r="A106" s="41" t="s">
         <v>127</v>
       </c>
       <c r="B106" s="26" t="s">
@@ -22663,7 +22744,7 @@
       <c r="Y106" s="27"/>
       <c r="Z106" s="27"/>
     </row>
-    <row r="107" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" s="102" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="52" t="s">
         <v>128</v>
       </c>
@@ -23536,7 +23617,7 @@
       <c r="Z126" s="27"/>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="57" t="s">
+      <c r="A127" s="56" t="s">
         <v>150</v>
       </c>
       <c r="B127" s="26" t="s">
@@ -23579,7 +23660,7 @@
       <c r="Y127" s="27"/>
       <c r="Z127" s="27"/>
     </row>
-    <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" s="47" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="58" t="s">
         <v>151</v>
       </c>
@@ -24051,53 +24132,41 @@
       <c r="Y138" s="27"/>
       <c r="Z138" s="27"/>
     </row>
-    <row r="139" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="62" t="s">
-        <v>162</v>
-      </c>
-      <c r="B139" s="63" t="s">
-        <v>16</v>
-      </c>
-      <c r="C139" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="D139" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="E139" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="F139" s="67" t="s">
-        <v>16</v>
-      </c>
-      <c r="G139" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="H139" s="69" t="s">
-        <v>16</v>
-      </c>
-      <c r="I139" s="65"/>
-      <c r="J139" s="70"/>
-      <c r="K139" s="64"/>
-      <c r="L139" s="64"/>
-      <c r="M139" s="64"/>
-      <c r="N139" s="64"/>
-      <c r="O139" s="64"/>
-      <c r="P139" s="64"/>
-      <c r="Q139" s="64"/>
-      <c r="R139" s="64"/>
-      <c r="S139" s="64"/>
-      <c r="T139" s="64"/>
-      <c r="U139" s="64"/>
-      <c r="V139" s="64"/>
-      <c r="W139" s="64"/>
-      <c r="X139" s="64"/>
-      <c r="Y139" s="64"/>
-      <c r="Z139" s="64"/>
+    <row r="139" spans="1:26" s="107" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="103" t="s">
+        <v>188</v>
+      </c>
+      <c r="B139" s="103"/>
+      <c r="C139" s="103"/>
+      <c r="D139" s="104"/>
+      <c r="E139" s="103"/>
+      <c r="F139" s="104"/>
+      <c r="G139" s="105"/>
+      <c r="H139" s="103"/>
+      <c r="I139" s="103"/>
+      <c r="J139" s="106"/>
+      <c r="K139" s="103" t="s">
+        <v>13</v>
+      </c>
+      <c r="L139" s="103"/>
+      <c r="M139" s="103"/>
+      <c r="N139" s="103"/>
+      <c r="O139" s="103"/>
+      <c r="P139" s="103"/>
+      <c r="Q139" s="103"/>
+      <c r="R139" s="103"/>
+      <c r="S139" s="103"/>
+      <c r="T139" s="103"/>
+      <c r="U139" s="103"/>
+      <c r="V139" s="103"/>
+      <c r="W139" s="103"/>
+      <c r="X139" s="103"/>
+      <c r="Y139" s="103"/>
+      <c r="Z139" s="103"/>
     </row>
     <row r="140" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="62" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B140" s="63" t="s">
         <v>16</v>
@@ -24139,9 +24208,9 @@
       <c r="Y140" s="64"/>
       <c r="Z140" s="64"/>
     </row>
-    <row r="141" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="62" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B141" s="63" t="s">
         <v>16</v>
@@ -24185,7 +24254,7 @@
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B142" s="63" t="s">
         <v>16</v>
@@ -24229,7 +24298,7 @@
     </row>
     <row r="143" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="62" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B143" s="63" t="s">
         <v>16</v>
@@ -24273,7 +24342,7 @@
     </row>
     <row r="144" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="62" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B144" s="63" t="s">
         <v>16</v>
@@ -24317,7 +24386,7 @@
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="62" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B145" s="63" t="s">
         <v>16</v>
@@ -24360,60 +24429,127 @@
       <c r="Z145" s="64"/>
     </row>
     <row r="146" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B146" s="71"/>
-      <c r="C146" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="E146" s="73"/>
-      <c r="F146" s="74"/>
-      <c r="H146" s="75"/>
-      <c r="K146" s="71"/>
-      <c r="L146" s="71"/>
-      <c r="M146" s="71"/>
-      <c r="N146" s="71"/>
-      <c r="O146" s="71"/>
-      <c r="P146" s="71"/>
-      <c r="Q146" s="71"/>
-      <c r="R146" s="71"/>
-    </row>
-    <row r="147" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B147" s="71"/>
-      <c r="C147" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="E147" s="73"/>
-      <c r="F147" s="74"/>
-      <c r="H147" s="75"/>
-      <c r="K147" s="71"/>
-      <c r="L147" s="71"/>
-      <c r="M147" s="71"/>
-      <c r="N147" s="71"/>
-      <c r="O147" s="71"/>
-      <c r="P147" s="71"/>
-      <c r="Q147" s="71"/>
-      <c r="R147" s="71"/>
-    </row>
-    <row r="148" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B148" s="71"/>
-      <c r="C148" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="E148" s="73"/>
-      <c r="F148" s="74"/>
-      <c r="H148" s="75"/>
-      <c r="K148" s="71"/>
-      <c r="L148" s="71"/>
-      <c r="M148" s="71"/>
-      <c r="N148" s="71"/>
-      <c r="O148" s="71"/>
-      <c r="P148" s="71"/>
-      <c r="Q148" s="71"/>
-      <c r="R148" s="71"/>
+      <c r="A146" s="62" t="s">
+        <v>168</v>
+      </c>
+      <c r="B146" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C146" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D146" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E146" s="66" t="s">
+        <v>16</v>
+      </c>
+      <c r="F146" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="G146" s="68" t="s">
+        <v>16</v>
+      </c>
+      <c r="H146" s="69" t="s">
+        <v>16</v>
+      </c>
+      <c r="I146" s="65"/>
+      <c r="J146" s="70"/>
+      <c r="K146" s="64"/>
+      <c r="L146" s="64"/>
+      <c r="M146" s="64"/>
+      <c r="N146" s="64"/>
+      <c r="O146" s="64"/>
+      <c r="P146" s="64"/>
+      <c r="Q146" s="64"/>
+      <c r="R146" s="64"/>
+      <c r="S146" s="64"/>
+      <c r="T146" s="64"/>
+      <c r="U146" s="64"/>
+      <c r="V146" s="64"/>
+      <c r="W146" s="64"/>
+      <c r="X146" s="64"/>
+      <c r="Y146" s="64"/>
+      <c r="Z146" s="64"/>
+    </row>
+    <row r="147" spans="1:26" s="101" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="97" t="s">
+        <v>186</v>
+      </c>
+      <c r="B147" s="97"/>
+      <c r="C147" s="97"/>
+      <c r="D147" s="98"/>
+      <c r="E147" s="97"/>
+      <c r="F147" s="98"/>
+      <c r="G147" s="99"/>
+      <c r="H147" s="97"/>
+      <c r="I147" s="97"/>
+      <c r="J147" s="100"/>
+      <c r="K147" s="97" t="s">
+        <v>13</v>
+      </c>
+      <c r="L147" s="97"/>
+      <c r="M147" s="97"/>
+      <c r="N147" s="97"/>
+      <c r="O147" s="97"/>
+      <c r="P147" s="97"/>
+      <c r="Q147" s="97"/>
+      <c r="R147" s="97"/>
+      <c r="S147" s="97"/>
+      <c r="T147" s="97"/>
+      <c r="U147" s="97"/>
+      <c r="V147" s="97"/>
+      <c r="W147" s="97"/>
+      <c r="X147" s="97"/>
+      <c r="Y147" s="97"/>
+      <c r="Z147" s="97"/>
+    </row>
+    <row r="148" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="B148" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D148" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E148" s="29">
+        <v>0</v>
+      </c>
+      <c r="F148" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G148" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H148" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I148" s="28"/>
+      <c r="J148" s="27"/>
+      <c r="K148" s="27"/>
+      <c r="L148" s="27"/>
+      <c r="M148" s="27"/>
+      <c r="N148" s="27"/>
+      <c r="O148" s="27"/>
+      <c r="P148" s="27"/>
+      <c r="Q148" s="27"/>
+      <c r="R148" s="27"/>
+      <c r="S148" s="27"/>
+      <c r="T148" s="27"/>
+      <c r="U148" s="27"/>
+      <c r="V148" s="27"/>
+      <c r="W148" s="27"/>
+      <c r="X148" s="27"/>
+      <c r="Y148" s="27"/>
+      <c r="Z148" s="27"/>
     </row>
     <row r="149" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B149" s="76" t="s">
-        <v>169</v>
-      </c>
+      <c r="B149" s="71"/>
       <c r="C149" s="72" t="s">
         <v>16</v>
       </c>
@@ -24429,10 +24565,8 @@
       <c r="Q149" s="71"/>
       <c r="R149" s="71"/>
     </row>
-    <row r="150" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B150" s="77" t="s">
-        <v>170</v>
-      </c>
+    <row r="150" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B150" s="71"/>
       <c r="C150" s="72" t="s">
         <v>16</v>
       </c>
@@ -24449,8 +24583,8 @@
       <c r="R150" s="71"/>
     </row>
     <row r="151" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B151" s="78" t="s">
-        <v>171</v>
+      <c r="B151" s="76" t="s">
+        <v>169</v>
       </c>
       <c r="C151" s="72" t="s">
         <v>16</v>
@@ -24468,6 +24602,9 @@
       <c r="R151" s="71"/>
     </row>
     <row r="152" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B152" s="77" t="s">
+        <v>170</v>
+      </c>
       <c r="C152" s="72" t="s">
         <v>16</v>
       </c>
@@ -24484,6 +24621,9 @@
       <c r="R152" s="71"/>
     </row>
     <row r="153" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B153" s="78" t="s">
+        <v>171</v>
+      </c>
       <c r="C153" s="72" t="s">
         <v>16</v>
       </c>
@@ -24515,7 +24655,7 @@
       <c r="Q154" s="71"/>
       <c r="R154" s="71"/>
     </row>
-    <row r="155" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C155" s="72" t="s">
         <v>16</v>
       </c>
@@ -24531,7 +24671,7 @@
       <c r="Q155" s="71"/>
       <c r="R155" s="71"/>
     </row>
-    <row r="156" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C156" s="72" t="s">
         <v>16</v>
       </c>
@@ -24579,7 +24719,7 @@
       <c r="Q158" s="71"/>
       <c r="R158" s="71"/>
     </row>
-    <row r="159" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C159" s="72" t="s">
         <v>16</v>
       </c>
@@ -25203,7 +25343,7 @@
       <c r="Q197" s="71"/>
       <c r="R197" s="71"/>
     </row>
-    <row r="198" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C198" s="72" t="s">
         <v>16</v>
       </c>
@@ -25219,7 +25359,7 @@
       <c r="Q198" s="71"/>
       <c r="R198" s="71"/>
     </row>
-    <row r="199" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C199" s="72" t="s">
         <v>16</v>
       </c>
@@ -26290,9 +26430,6 @@
       <c r="P265" s="71"/>
       <c r="Q265" s="71"/>
       <c r="R265" s="71"/>
-      <c r="X265" s="79"/>
-      <c r="Y265" s="79"/>
-      <c r="Z265" s="79"/>
     </row>
     <row r="266" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C266" s="72" t="s">
@@ -26325,6 +26462,9 @@
       <c r="P267" s="71"/>
       <c r="Q267" s="71"/>
       <c r="R267" s="71"/>
+      <c r="X267" s="79"/>
+      <c r="Y267" s="79"/>
+      <c r="Z267" s="79"/>
     </row>
     <row r="268" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C268" s="72" t="s">
@@ -26389,9 +26529,6 @@
       <c r="P271" s="71"/>
       <c r="Q271" s="71"/>
       <c r="R271" s="71"/>
-      <c r="X271" s="79"/>
-      <c r="Y271" s="79"/>
-      <c r="Z271" s="79"/>
     </row>
     <row r="272" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C272" s="72" t="s">
@@ -26409,7 +26546,7 @@
       <c r="Q272" s="71"/>
       <c r="R272" s="71"/>
     </row>
-    <row r="273" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C273" s="72" t="s">
         <v>16</v>
       </c>
@@ -26424,8 +26561,11 @@
       <c r="P273" s="71"/>
       <c r="Q273" s="71"/>
       <c r="R273" s="71"/>
-    </row>
-    <row r="274" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X273" s="79"/>
+      <c r="Y273" s="79"/>
+      <c r="Z273" s="79"/>
+    </row>
+    <row r="274" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C274" s="72" t="s">
         <v>16</v>
       </c>
@@ -26441,7 +26581,7 @@
       <c r="Q274" s="71"/>
       <c r="R274" s="71"/>
     </row>
-    <row r="275" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C275" s="72" t="s">
         <v>16</v>
       </c>
@@ -26457,7 +26597,7 @@
       <c r="Q275" s="71"/>
       <c r="R275" s="71"/>
     </row>
-    <row r="276" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C276" s="72" t="s">
         <v>16</v>
       </c>
@@ -26473,7 +26613,7 @@
       <c r="Q276" s="71"/>
       <c r="R276" s="71"/>
     </row>
-    <row r="277" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C277" s="72" t="s">
         <v>16</v>
       </c>
@@ -26489,7 +26629,7 @@
       <c r="Q277" s="71"/>
       <c r="R277" s="71"/>
     </row>
-    <row r="278" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C278" s="72" t="s">
         <v>16</v>
       </c>
@@ -26505,7 +26645,7 @@
       <c r="Q278" s="71"/>
       <c r="R278" s="71"/>
     </row>
-    <row r="279" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C279" s="72" t="s">
         <v>16</v>
       </c>
@@ -26521,7 +26661,7 @@
       <c r="Q279" s="71"/>
       <c r="R279" s="71"/>
     </row>
-    <row r="280" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C280" s="72" t="s">
         <v>16</v>
       </c>
@@ -26537,7 +26677,7 @@
       <c r="Q280" s="71"/>
       <c r="R280" s="71"/>
     </row>
-    <row r="281" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C281" s="72" t="s">
         <v>16</v>
       </c>
@@ -26553,7 +26693,7 @@
       <c r="Q281" s="71"/>
       <c r="R281" s="71"/>
     </row>
-    <row r="282" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C282" s="72" t="s">
         <v>16</v>
       </c>
@@ -26569,7 +26709,7 @@
       <c r="Q282" s="71"/>
       <c r="R282" s="71"/>
     </row>
-    <row r="283" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C283" s="72" t="s">
         <v>16</v>
       </c>
@@ -26585,7 +26725,7 @@
       <c r="Q283" s="71"/>
       <c r="R283" s="71"/>
     </row>
-    <row r="284" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C284" s="72" t="s">
         <v>16</v>
       </c>
@@ -26601,7 +26741,7 @@
       <c r="Q284" s="71"/>
       <c r="R284" s="71"/>
     </row>
-    <row r="285" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C285" s="72" t="s">
         <v>16</v>
       </c>
@@ -26617,7 +26757,7 @@
       <c r="Q285" s="71"/>
       <c r="R285" s="71"/>
     </row>
-    <row r="286" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C286" s="72" t="s">
         <v>16</v>
       </c>
@@ -26633,7 +26773,7 @@
       <c r="Q286" s="71"/>
       <c r="R286" s="71"/>
     </row>
-    <row r="287" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C287" s="72" t="s">
         <v>16</v>
       </c>
@@ -26649,7 +26789,7 @@
       <c r="Q287" s="71"/>
       <c r="R287" s="71"/>
     </row>
-    <row r="288" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="3:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C288" s="72" t="s">
         <v>16</v>
       </c>
@@ -27056,6 +27196,7 @@
       <c r="E313" s="73"/>
       <c r="F313" s="74"/>
       <c r="H313" s="75"/>
+      <c r="K313" s="71"/>
       <c r="L313" s="71"/>
       <c r="M313" s="71"/>
       <c r="N313" s="71"/>
@@ -27071,6 +27212,14 @@
       <c r="E314" s="73"/>
       <c r="F314" s="74"/>
       <c r="H314" s="75"/>
+      <c r="K314" s="71"/>
+      <c r="L314" s="71"/>
+      <c r="M314" s="71"/>
+      <c r="N314" s="71"/>
+      <c r="O314" s="71"/>
+      <c r="P314" s="71"/>
+      <c r="Q314" s="71"/>
+      <c r="R314" s="71"/>
     </row>
     <row r="315" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C315" s="72" t="s">
@@ -27079,6 +27228,13 @@
       <c r="E315" s="73"/>
       <c r="F315" s="74"/>
       <c r="H315" s="75"/>
+      <c r="L315" s="71"/>
+      <c r="M315" s="71"/>
+      <c r="N315" s="71"/>
+      <c r="O315" s="71"/>
+      <c r="P315" s="71"/>
+      <c r="Q315" s="71"/>
+      <c r="R315" s="71"/>
     </row>
     <row r="316" spans="3:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C316" s="72" t="s">
@@ -27616,7 +27772,7 @@
       <c r="F382" s="74"/>
       <c r="H382" s="75"/>
     </row>
-    <row r="383" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C383" s="72" t="s">
         <v>16</v>
       </c>
@@ -27632,7 +27788,7 @@
       <c r="F384" s="74"/>
       <c r="H384" s="75"/>
     </row>
-    <row r="385" spans="3:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="3:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C385" s="72" t="s">
         <v>16</v>
       </c>
@@ -31881,85 +32037,79 @@
       <c r="H915" s="75"/>
     </row>
     <row r="916" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C916" s="80" t="s">
+      <c r="C916" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E916" s="73"/>
+      <c r="F916" s="74"/>
+      <c r="H916" s="75"/>
+    </row>
+    <row r="917" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C917" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="E917" s="73"/>
+      <c r="F917" s="74"/>
+      <c r="H917" s="75"/>
+    </row>
+    <row r="918" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C918" s="80" t="s">
         <v>172</v>
       </c>
-      <c r="D916" s="81" t="s">
+      <c r="D918" s="81" t="s">
         <v>173</v>
       </c>
-      <c r="E916" s="82">
+      <c r="E918" s="82">
         <v>1</v>
       </c>
-      <c r="F916" s="83" t="s">
-        <v>15</v>
-      </c>
-      <c r="G916" s="84" t="s">
+      <c r="F918" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="G918" s="84" t="s">
         <v>174</v>
       </c>
-      <c r="H916" s="85" t="s">
+      <c r="H918" s="85" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="917" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B917" s="71" t="s">
+    <row r="919" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B919" s="71" t="s">
         <v>176</v>
       </c>
-      <c r="C917" s="72" t="s">
+      <c r="C919" s="72" t="s">
         <v>172</v>
       </c>
-      <c r="D917" s="71"/>
-      <c r="E917" s="73">
+      <c r="D919" s="71"/>
+      <c r="E919" s="73">
         <v>3</v>
       </c>
-      <c r="F917" s="74"/>
-      <c r="G917" s="86" t="s">
+      <c r="F919" s="74"/>
+      <c r="G919" s="86" t="s">
         <v>177</v>
       </c>
-      <c r="H917" s="87"/>
-    </row>
-    <row r="918" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B918" s="71" t="s">
+      <c r="H919" s="87"/>
+    </row>
+    <row r="920" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B920" s="71" t="s">
         <v>178</v>
       </c>
-      <c r="C918" s="8" t="s">
+      <c r="C920" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E918" s="73" t="s">
+      <c r="E920" s="73" t="s">
         <v>179</v>
       </c>
-      <c r="F918" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="G918" s="88" t="s">
+      <c r="F920" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="G920" s="88" t="s">
         <v>180</v>
       </c>
-      <c r="H918" s="75"/>
-      <c r="J918" s="89" t="s">
+      <c r="H920" s="75"/>
+      <c r="J920" s="89" t="s">
         <v>181</v>
       </c>
-      <c r="K918" s="71"/>
-    </row>
-    <row r="919" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B919" s="71"/>
-      <c r="C919" s="71"/>
-      <c r="D919" s="71"/>
-      <c r="E919" s="71"/>
-      <c r="F919" s="71"/>
-      <c r="G919" s="86"/>
-      <c r="H919" s="71"/>
-      <c r="I919" s="71"/>
-      <c r="J919" s="90"/>
-    </row>
-    <row r="920" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B920" s="71"/>
-      <c r="C920" s="71"/>
-      <c r="D920" s="71"/>
-      <c r="E920" s="71"/>
-      <c r="F920" s="71"/>
-      <c r="G920" s="86"/>
-      <c r="H920" s="71"/>
-      <c r="I920" s="71"/>
-      <c r="J920" s="90"/>
+      <c r="K920" s="71"/>
     </row>
     <row r="921" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B921" s="71"/>
@@ -32005,8 +32155,28 @@
       <c r="I924" s="71"/>
       <c r="J924" s="90"/>
     </row>
-    <row r="925" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="926" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="925" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B925" s="71"/>
+      <c r="C925" s="71"/>
+      <c r="D925" s="71"/>
+      <c r="E925" s="71"/>
+      <c r="F925" s="71"/>
+      <c r="G925" s="86"/>
+      <c r="H925" s="71"/>
+      <c r="I925" s="71"/>
+      <c r="J925" s="90"/>
+    </row>
+    <row r="926" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B926" s="71"/>
+      <c r="C926" s="71"/>
+      <c r="D926" s="71"/>
+      <c r="E926" s="71"/>
+      <c r="F926" s="71"/>
+      <c r="G926" s="86"/>
+      <c r="H926" s="71"/>
+      <c r="I926" s="71"/>
+      <c r="J926" s="90"/>
+    </row>
     <row r="927" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="928" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="929" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32021,17 +32191,17 @@
     <row r="938" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="939" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="940" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="941" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A941" s="8"/>
-      <c r="B941" s="91" t="s">
+    <row r="941" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="942" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="943" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A943" s="8"/>
+      <c r="B943" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="I941" s="92" t="s">
+      <c r="I943" s="92" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="942" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="943" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="944" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="945" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="946" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32039,49 +32209,39 @@
     <row r="948" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="949" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="950" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="951" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B951" s="28"/>
-      <c r="C951" s="27"/>
-      <c r="D951" s="28"/>
-      <c r="E951" s="29"/>
-      <c r="F951" s="30"/>
-      <c r="G951" s="93" t="s">
-        <v>184</v>
-      </c>
-      <c r="H951" s="31"/>
-      <c r="I951" s="28"/>
-      <c r="J951" s="94"/>
-    </row>
+    <row r="951" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="952" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="953" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B953" s="1"/>
-      <c r="E953" s="1"/>
-      <c r="F953" s="2"/>
-      <c r="G953" s="95"/>
-      <c r="H953" s="1"/>
+      <c r="B953" s="28"/>
+      <c r="C953" s="27"/>
+      <c r="D953" s="28"/>
+      <c r="E953" s="29"/>
+      <c r="F953" s="30"/>
+      <c r="G953" s="93" t="s">
+        <v>184</v>
+      </c>
+      <c r="H953" s="31"/>
+      <c r="I953" s="28"/>
+      <c r="J953" s="94"/>
     </row>
     <row r="954" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="955" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B955" s="28"/>
-      <c r="C955" s="27"/>
-      <c r="D955" s="28"/>
-      <c r="E955" s="29"/>
-      <c r="F955" s="30"/>
-      <c r="G955" s="96"/>
-      <c r="H955" s="31"/>
-      <c r="I955" s="28"/>
-      <c r="J955" s="94"/>
-    </row>
-    <row r="956" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E956" s="1"/>
-      <c r="F956" s="2"/>
-      <c r="H956" s="2"/>
-      <c r="J956" s="94"/>
-    </row>
+      <c r="B955" s="1"/>
+      <c r="E955" s="1"/>
+      <c r="F955" s="2"/>
+      <c r="G955" s="95"/>
+      <c r="H955" s="1"/>
+    </row>
+    <row r="956" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="957" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E957" s="1"/>
-      <c r="F957" s="2"/>
-      <c r="H957" s="2"/>
+      <c r="B957" s="28"/>
+      <c r="C957" s="27"/>
+      <c r="D957" s="28"/>
+      <c r="E957" s="29"/>
+      <c r="F957" s="30"/>
+      <c r="G957" s="96"/>
+      <c r="H957" s="31"/>
+      <c r="I957" s="28"/>
       <c r="J957" s="94"/>
     </row>
     <row r="958" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -32103,11 +32263,9 @@
       <c r="J960" s="94"/>
     </row>
     <row r="961" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B961" s="1"/>
       <c r="E961" s="1"/>
       <c r="F961" s="2"/>
-      <c r="G961" s="95"/>
-      <c r="H961" s="1"/>
+      <c r="H961" s="2"/>
       <c r="J961" s="94"/>
     </row>
     <row r="962" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -32117,9 +32275,11 @@
       <c r="J962" s="94"/>
     </row>
     <row r="963" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B963" s="1"/>
       <c r="E963" s="1"/>
       <c r="F963" s="2"/>
-      <c r="H963" s="2"/>
+      <c r="G963" s="95"/>
+      <c r="H963" s="1"/>
       <c r="J963" s="94"/>
     </row>
     <row r="964" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -32147,11 +32307,9 @@
       <c r="J967" s="94"/>
     </row>
     <row r="968" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B968" s="1"/>
       <c r="E968" s="1"/>
       <c r="F968" s="2"/>
-      <c r="G968" s="95"/>
-      <c r="H968" s="1"/>
+      <c r="H968" s="2"/>
       <c r="J968" s="94"/>
     </row>
     <row r="969" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -32175,9 +32333,11 @@
       <c r="J971" s="94"/>
     </row>
     <row r="972" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B972" s="1"/>
       <c r="E972" s="1"/>
       <c r="F972" s="2"/>
-      <c r="H972" s="2"/>
+      <c r="G972" s="95"/>
+      <c r="H972" s="1"/>
       <c r="J972" s="94"/>
     </row>
     <row r="973" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -32235,68 +32395,53 @@
       <c r="J981" s="94"/>
     </row>
     <row r="982" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B982" s="1"/>
       <c r="E982" s="1"/>
       <c r="F982" s="2"/>
-      <c r="G982" s="95"/>
-      <c r="H982" s="1"/>
+      <c r="H982" s="2"/>
       <c r="J982" s="94"/>
     </row>
     <row r="983" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B983" s="1"/>
       <c r="E983" s="1"/>
       <c r="F983" s="2"/>
-      <c r="G983" s="95"/>
-      <c r="H983" s="1"/>
+      <c r="H983" s="2"/>
       <c r="J983" s="94"/>
     </row>
-    <row r="984" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="984" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B984" s="1"/>
+      <c r="E984" s="1"/>
+      <c r="F984" s="2"/>
+      <c r="G984" s="95"/>
+      <c r="H984" s="1"/>
+      <c r="J984" s="94"/>
+    </row>
+    <row r="985" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B985" s="1"/>
+      <c r="E985" s="1"/>
+      <c r="F985" s="2"/>
+      <c r="G985" s="95"/>
+      <c r="H985" s="1"/>
+      <c r="J985" s="94"/>
+    </row>
     <row r="986" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="987" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="988" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="989" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="990" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B991" s="1"/>
-      <c r="E991" s="1"/>
-      <c r="F991" s="2"/>
-      <c r="G991" s="95"/>
-      <c r="H991" s="1"/>
-      <c r="J991" s="94"/>
-    </row>
+    <row r="991" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="992" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="993" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E993" s="73"/>
-      <c r="F993" s="74"/>
-      <c r="H993" s="75"/>
-    </row>
-    <row r="994" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A994" s="72"/>
-      <c r="B994" s="71"/>
-      <c r="C994" s="71"/>
-      <c r="D994" s="71"/>
-      <c r="E994" s="71"/>
-      <c r="F994" s="71"/>
-      <c r="G994" s="86"/>
-      <c r="H994" s="71"/>
-      <c r="I994" s="71"/>
-      <c r="J994" s="90"/>
-      <c r="K994" s="8" t="s">
-        <v>183</v>
-      </c>
-    </row>
+      <c r="B993" s="1"/>
+      <c r="E993" s="1"/>
+      <c r="F993" s="2"/>
+      <c r="G993" s="95"/>
+      <c r="H993" s="1"/>
+      <c r="J993" s="94"/>
+    </row>
+    <row r="994" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="995" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A995" s="72"/>
-      <c r="B995" s="71"/>
-      <c r="C995" s="71"/>
-      <c r="D995" s="71"/>
-      <c r="E995" s="71"/>
-      <c r="F995" s="71"/>
-      <c r="G995" s="86"/>
-      <c r="H995" s="71"/>
-      <c r="I995" s="71"/>
-      <c r="J995" s="90"/>
+      <c r="E995" s="73"/>
+      <c r="F995" s="74"/>
+      <c r="H995" s="75"/>
     </row>
     <row r="996" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A996" s="72"/>
@@ -32309,6 +32454,9 @@
       <c r="H996" s="71"/>
       <c r="I996" s="71"/>
       <c r="J996" s="90"/>
+      <c r="K996" s="8" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="997" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A997" s="72"/>
@@ -33414,7 +33562,7 @@
       <c r="I1088" s="71"/>
       <c r="J1088" s="90"/>
     </row>
-    <row r="1089" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1089" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1089" s="72"/>
       <c r="B1089" s="71"/>
       <c r="C1089" s="71"/>
@@ -33438,7 +33586,7 @@
       <c r="I1090" s="71"/>
       <c r="J1090" s="90"/>
     </row>
-    <row r="1091" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1091" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1091" s="72"/>
       <c r="B1091" s="71"/>
       <c r="C1091" s="71"/>
@@ -33713,22 +33861,6 @@
       <c r="H1113" s="71"/>
       <c r="I1113" s="71"/>
       <c r="J1113" s="90"/>
-      <c r="K1113" s="27"/>
-      <c r="L1113" s="27"/>
-      <c r="M1113" s="27"/>
-      <c r="N1113" s="27"/>
-      <c r="O1113" s="27"/>
-      <c r="P1113" s="27"/>
-      <c r="Q1113" s="27"/>
-      <c r="R1113" s="27"/>
-      <c r="S1113" s="27"/>
-      <c r="T1113" s="27"/>
-      <c r="U1113" s="27"/>
-      <c r="V1113" s="27"/>
-      <c r="W1113" s="27"/>
-      <c r="X1113" s="27"/>
-      <c r="Y1113" s="27"/>
-      <c r="Z1113" s="27"/>
     </row>
     <row r="1114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1114" s="72"/>
@@ -33753,6 +33885,22 @@
       <c r="H1115" s="71"/>
       <c r="I1115" s="71"/>
       <c r="J1115" s="90"/>
+      <c r="K1115" s="27"/>
+      <c r="L1115" s="27"/>
+      <c r="M1115" s="27"/>
+      <c r="N1115" s="27"/>
+      <c r="O1115" s="27"/>
+      <c r="P1115" s="27"/>
+      <c r="Q1115" s="27"/>
+      <c r="R1115" s="27"/>
+      <c r="S1115" s="27"/>
+      <c r="T1115" s="27"/>
+      <c r="U1115" s="27"/>
+      <c r="V1115" s="27"/>
+      <c r="W1115" s="27"/>
+      <c r="X1115" s="27"/>
+      <c r="Y1115" s="27"/>
+      <c r="Z1115" s="27"/>
     </row>
     <row r="1116" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1116" s="72"/>
@@ -33946,7 +34094,7 @@
       <c r="I1131" s="71"/>
       <c r="J1131" s="90"/>
     </row>
-    <row r="1132" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1132" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1132" s="72"/>
       <c r="B1132" s="71"/>
       <c r="C1132" s="71"/>
@@ -33958,7 +34106,7 @@
       <c r="I1132" s="71"/>
       <c r="J1132" s="90"/>
     </row>
-    <row r="1133" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1133" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1133" s="72"/>
       <c r="B1133" s="71"/>
       <c r="C1133" s="71"/>
@@ -34234,11 +34382,35 @@
       <c r="I1155" s="71"/>
       <c r="J1155" s="90"/>
     </row>
+    <row r="1156" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1156" s="72"/>
+      <c r="B1156" s="71"/>
+      <c r="C1156" s="71"/>
+      <c r="D1156" s="71"/>
+      <c r="E1156" s="71"/>
+      <c r="F1156" s="71"/>
+      <c r="G1156" s="86"/>
+      <c r="H1156" s="71"/>
+      <c r="I1156" s="71"/>
+      <c r="J1156" s="90"/>
+    </row>
+    <row r="1157" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1157" s="72"/>
+      <c r="B1157" s="71"/>
+      <c r="C1157" s="71"/>
+      <c r="D1157" s="71"/>
+      <c r="E1157" s="71"/>
+      <c r="F1157" s="71"/>
+      <c r="G1157" s="86"/>
+      <c r="H1157" s="71"/>
+      <c r="I1157" s="71"/>
+      <c r="J1157" s="90"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <phoneticPr fontId="24" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C66:C85 C45:C64 C3:C22 C299 C289 C287 C278 C276 C274 C263:C264 C261 C259 C248:C249 C246 C244 C24:C43 C235 C233 C231 C222 C213 C210:C211 C208 C206 C178:C179 C176 C174 C129:C145 C108:C127 C325:C1155 C87:C106" xr:uid="{DF59C5D8-C83E-40D2-AFC8-A093518F80A5}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C66:C85 C45:C64 C3:C22 C301 C291 C289 C280 C278 C276 C265:C266 C263 C261 C250:C251 C248 C246 C24:C43 C237 C235 C233 C224 C215 C212:C213 C210 C208 C180:C181 C178 C176 C87:C106 C108:C127 C327:C1157 C129:C138 C140:C146 C148" xr:uid="{DF59C5D8-C83E-40D2-AFC8-A093518F80A5}">
       <formula1>"Hero,Unit,Event,Twist,Dream,Equipment,Member,Token,- - -"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Description is being processed
</commit_message>
<xml_diff>
--- a/TestSheet.xlsx
+++ b/TestSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_09CE59F3B32C71B27447F41703FFAE311A56176B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25E90753-C37E-40A0-BE4D-959040AE3F19}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="11_09CE59F3B32C71B27447F41703FFAE311A56176B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBB6532C-CB74-410F-B275-4D55BA31A760}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1035" yWindow="1470" windowWidth="18210" windowHeight="10965" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pack Template" sheetId="11" state="hidden" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1651,6 +1651,8 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18109,8 +18111,8 @@
   <dimension ref="A1:Z1157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G97" sqref="G97"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18201,7 +18203,7 @@
       <c r="Z2" s="20"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="26" t="s">
@@ -18245,7 +18247,7 @@
       <c r="Z3" s="27"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="26" t="s">
@@ -18289,7 +18291,7 @@
       <c r="Z4" s="27"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="26" t="s">
@@ -18333,7 +18335,7 @@
       <c r="Z5" s="27"/>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="26" t="s">
@@ -18377,7 +18379,7 @@
       <c r="Z6" s="27"/>
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="26" t="s">
@@ -18421,7 +18423,7 @@
       <c r="Z7" s="27"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="26" t="s">
@@ -18465,7 +18467,7 @@
       <c r="Z8" s="27"/>
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="26" t="s">
@@ -18509,7 +18511,7 @@
       <c r="Z9" s="27"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="26" t="s">
@@ -18553,7 +18555,7 @@
       <c r="Z10" s="27"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="26" t="s">
@@ -18597,7 +18599,7 @@
       <c r="Z11" s="27"/>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="26" t="s">
@@ -18641,7 +18643,7 @@
       <c r="Z12" s="27"/>
     </row>
     <row r="13" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="26" t="s">
@@ -18685,7 +18687,7 @@
       <c r="Z13" s="27"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -18729,7 +18731,7 @@
       <c r="Z14" s="27"/>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="26" t="s">
@@ -18773,7 +18775,7 @@
       <c r="Z15" s="27"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="26" t="s">
@@ -18817,7 +18819,7 @@
       <c r="Z16" s="27"/>
     </row>
     <row r="17" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="26" t="s">
@@ -18861,7 +18863,7 @@
       <c r="Z17" s="27"/>
     </row>
     <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B18" s="26" t="s">
@@ -18905,7 +18907,7 @@
       <c r="Z18" s="27"/>
     </row>
     <row r="19" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="26" t="s">
@@ -18949,7 +18951,7 @@
       <c r="Z19" s="27"/>
     </row>
     <row r="20" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="26" t="s">
@@ -18993,7 +18995,7 @@
       <c r="Z20" s="27"/>
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B21" s="26" t="s">
@@ -19037,7 +19039,7 @@
       <c r="Z21" s="27"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="26" t="s">
@@ -19117,7 +19119,7 @@
       <c r="Z23" s="33"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="26" t="s">
@@ -19161,7 +19163,7 @@
       <c r="Z24" s="27"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="26" t="s">
@@ -19205,7 +19207,7 @@
       <c r="Z25" s="27"/>
     </row>
     <row r="26" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="26" t="s">
@@ -19249,7 +19251,7 @@
       <c r="Z26" s="27"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="26" t="s">
@@ -19293,7 +19295,7 @@
       <c r="Z27" s="27"/>
     </row>
     <row r="28" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="26" t="s">
@@ -19337,7 +19339,7 @@
       <c r="Z28" s="27"/>
     </row>
     <row r="29" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="26" t="s">
@@ -19381,7 +19383,7 @@
       <c r="Z29" s="27"/>
     </row>
     <row r="30" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B30" s="26" t="s">
@@ -19425,7 +19427,7 @@
       <c r="Z30" s="27"/>
     </row>
     <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="26" t="s">
@@ -19469,7 +19471,7 @@
       <c r="Z31" s="27"/>
     </row>
     <row r="32" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B32" s="26" t="s">
@@ -19513,7 +19515,7 @@
       <c r="Z32" s="27"/>
     </row>
     <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B33" s="26" t="s">
@@ -19557,7 +19559,7 @@
       <c r="Z33" s="27"/>
     </row>
     <row r="34" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="26" t="s">
@@ -19601,7 +19603,7 @@
       <c r="Z34" s="27"/>
     </row>
     <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B35" s="26" t="s">
@@ -19645,7 +19647,7 @@
       <c r="Z35" s="27"/>
     </row>
     <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B36" s="26" t="s">
@@ -19689,7 +19691,7 @@
       <c r="Z36" s="27"/>
     </row>
     <row r="37" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B37" s="26" t="s">
@@ -19733,7 +19735,7 @@
       <c r="Z37" s="27"/>
     </row>
     <row r="38" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B38" s="26" t="s">
@@ -19777,7 +19779,7 @@
       <c r="Z38" s="27"/>
     </row>
     <row r="39" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B39" s="26" t="s">
@@ -19821,7 +19823,7 @@
       <c r="Z39" s="27"/>
     </row>
     <row r="40" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="26" t="s">
@@ -19865,7 +19867,7 @@
       <c r="Z40" s="27"/>
     </row>
     <row r="41" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="8" t="s">
         <v>56</v>
       </c>
       <c r="B41" s="26" t="s">
@@ -19909,7 +19911,7 @@
       <c r="Z41" s="27"/>
     </row>
     <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B42" s="26" t="s">
@@ -19953,7 +19955,7 @@
       <c r="Z42" s="27"/>
     </row>
     <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B43" s="26" t="s">
@@ -20033,7 +20035,7 @@
       <c r="Z44" s="37"/>
     </row>
     <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="108" t="s">
         <v>62</v>
       </c>
       <c r="B45" s="26" t="s">
@@ -20077,7 +20079,7 @@
       <c r="Z45" s="27"/>
     </row>
     <row r="46" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="41" t="s">
+      <c r="A46" s="108" t="s">
         <v>63</v>
       </c>
       <c r="B46" s="26" t="s">
@@ -20121,7 +20123,7 @@
       <c r="Z46" s="27"/>
     </row>
     <row r="47" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="108" t="s">
         <v>64</v>
       </c>
       <c r="B47" s="26" t="s">
@@ -20165,7 +20167,7 @@
       <c r="Z47" s="27"/>
     </row>
     <row r="48" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="108" t="s">
         <v>65</v>
       </c>
       <c r="B48" s="26" t="s">
@@ -20209,7 +20211,7 @@
       <c r="Z48" s="27"/>
     </row>
     <row r="49" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="41" t="s">
+      <c r="A49" s="108" t="s">
         <v>66</v>
       </c>
       <c r="B49" s="26" t="s">
@@ -20253,7 +20255,7 @@
       <c r="Z49" s="27"/>
     </row>
     <row r="50" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="108" t="s">
         <v>67</v>
       </c>
       <c r="B50" s="26" t="s">
@@ -20297,7 +20299,7 @@
       <c r="Z50" s="27"/>
     </row>
     <row r="51" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="41" t="s">
+      <c r="A51" s="108" t="s">
         <v>68</v>
       </c>
       <c r="B51" s="26" t="s">
@@ -20341,7 +20343,7 @@
       <c r="Z51" s="27"/>
     </row>
     <row r="52" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="41" t="s">
+      <c r="A52" s="108" t="s">
         <v>69</v>
       </c>
       <c r="B52" s="26" t="s">
@@ -20385,7 +20387,7 @@
       <c r="Z52" s="27"/>
     </row>
     <row r="53" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="108" t="s">
         <v>70</v>
       </c>
       <c r="B53" s="26" t="s">
@@ -20429,7 +20431,7 @@
       <c r="Z53" s="27"/>
     </row>
     <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="41" t="s">
+      <c r="A54" s="108" t="s">
         <v>71</v>
       </c>
       <c r="B54" s="26" t="s">
@@ -20473,7 +20475,7 @@
       <c r="Z54" s="27"/>
     </row>
     <row r="55" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="41" t="s">
+      <c r="A55" s="108" t="s">
         <v>72</v>
       </c>
       <c r="B55" s="26" t="s">
@@ -20517,7 +20519,7 @@
       <c r="Z55" s="27"/>
     </row>
     <row r="56" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="41" t="s">
+      <c r="A56" s="108" t="s">
         <v>73</v>
       </c>
       <c r="B56" s="26" t="s">
@@ -20561,7 +20563,7 @@
       <c r="Z56" s="27"/>
     </row>
     <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="41" t="s">
+      <c r="A57" s="108" t="s">
         <v>74</v>
       </c>
       <c r="B57" s="26" t="s">
@@ -20605,7 +20607,7 @@
       <c r="Z57" s="27"/>
     </row>
     <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="41" t="s">
+      <c r="A58" s="108" t="s">
         <v>75</v>
       </c>
       <c r="B58" s="26" t="s">
@@ -20649,7 +20651,7 @@
       <c r="Z58" s="27"/>
     </row>
     <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="41" t="s">
+      <c r="A59" s="108" t="s">
         <v>76</v>
       </c>
       <c r="B59" s="26" t="s">
@@ -20693,7 +20695,7 @@
       <c r="Z59" s="27"/>
     </row>
     <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="108" t="s">
         <v>77</v>
       </c>
       <c r="B60" s="26" t="s">
@@ -20737,7 +20739,7 @@
       <c r="Z60" s="27"/>
     </row>
     <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="41" t="s">
+      <c r="A61" s="108" t="s">
         <v>78</v>
       </c>
       <c r="B61" s="26" t="s">
@@ -20781,7 +20783,7 @@
       <c r="Z61" s="27"/>
     </row>
     <row r="62" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="41" t="s">
+      <c r="A62" s="108" t="s">
         <v>79</v>
       </c>
       <c r="B62" s="26" t="s">
@@ -20825,7 +20827,7 @@
       <c r="Z62" s="27"/>
     </row>
     <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="41" t="s">
+      <c r="A63" s="108" t="s">
         <v>80</v>
       </c>
       <c r="B63" s="26" t="s">
@@ -20869,7 +20871,7 @@
       <c r="Z63" s="27"/>
     </row>
     <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="108" t="s">
         <v>81</v>
       </c>
       <c r="B64" s="26" t="s">
@@ -20949,7 +20951,7 @@
       <c r="Z65" s="43"/>
     </row>
     <row r="66" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="41" t="s">
+      <c r="A66" s="108" t="s">
         <v>85</v>
       </c>
       <c r="B66" s="26" t="s">
@@ -20993,7 +20995,7 @@
       <c r="Z66" s="27"/>
     </row>
     <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="108" t="s">
         <v>86</v>
       </c>
       <c r="B67" s="26" t="s">
@@ -21037,7 +21039,7 @@
       <c r="Z67" s="27"/>
     </row>
     <row r="68" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="41" t="s">
+      <c r="A68" s="108" t="s">
         <v>87</v>
       </c>
       <c r="B68" s="26" t="s">
@@ -21081,7 +21083,7 @@
       <c r="Z68" s="27"/>
     </row>
     <row r="69" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="41" t="s">
+      <c r="A69" s="108" t="s">
         <v>88</v>
       </c>
       <c r="B69" s="26" t="s">
@@ -21125,7 +21127,7 @@
       <c r="Z69" s="27"/>
     </row>
     <row r="70" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="108" t="s">
         <v>89</v>
       </c>
       <c r="B70" s="26" t="s">
@@ -21169,7 +21171,7 @@
       <c r="Z70" s="27"/>
     </row>
     <row r="71" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="41" t="s">
+      <c r="A71" s="108" t="s">
         <v>90</v>
       </c>
       <c r="B71" s="26" t="s">
@@ -21213,7 +21215,7 @@
       <c r="Z71" s="27"/>
     </row>
     <row r="72" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="108" t="s">
         <v>91</v>
       </c>
       <c r="B72" s="26" t="s">
@@ -21257,7 +21259,7 @@
       <c r="Z72" s="27"/>
     </row>
     <row r="73" spans="1:26" s="47" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="41" t="s">
+      <c r="A73" s="108" t="s">
         <v>92</v>
       </c>
       <c r="B73" s="26" t="s">
@@ -21301,7 +21303,7 @@
       <c r="Z73" s="27"/>
     </row>
     <row r="74" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="41" t="s">
+      <c r="A74" s="108" t="s">
         <v>93</v>
       </c>
       <c r="B74" s="26" t="s">
@@ -21345,7 +21347,7 @@
       <c r="Z74" s="27"/>
     </row>
     <row r="75" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="41" t="s">
+      <c r="A75" s="108" t="s">
         <v>94</v>
       </c>
       <c r="B75" s="26" t="s">
@@ -21389,7 +21391,7 @@
       <c r="Z75" s="27"/>
     </row>
     <row r="76" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="41" t="s">
+      <c r="A76" s="108" t="s">
         <v>95</v>
       </c>
       <c r="B76" s="26" t="s">
@@ -21433,7 +21435,7 @@
       <c r="Z76" s="27"/>
     </row>
     <row r="77" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="108" t="s">
         <v>96</v>
       </c>
       <c r="B77" s="26" t="s">
@@ -21477,7 +21479,7 @@
       <c r="Z77" s="27"/>
     </row>
     <row r="78" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="41" t="s">
+      <c r="A78" s="108" t="s">
         <v>97</v>
       </c>
       <c r="B78" s="26" t="s">
@@ -21521,7 +21523,7 @@
       <c r="Z78" s="27"/>
     </row>
     <row r="79" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="108" t="s">
         <v>98</v>
       </c>
       <c r="B79" s="26" t="s">
@@ -21565,7 +21567,7 @@
       <c r="Z79" s="27"/>
     </row>
     <row r="80" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="108" t="s">
         <v>99</v>
       </c>
       <c r="B80" s="26" t="s">
@@ -21609,7 +21611,7 @@
       <c r="Z80" s="27"/>
     </row>
     <row r="81" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="41" t="s">
+      <c r="A81" s="108" t="s">
         <v>100</v>
       </c>
       <c r="B81" s="26" t="s">
@@ -21653,7 +21655,7 @@
       <c r="Z81" s="27"/>
     </row>
     <row r="82" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="41" t="s">
+      <c r="A82" s="108" t="s">
         <v>101</v>
       </c>
       <c r="B82" s="26" t="s">
@@ -21697,7 +21699,7 @@
       <c r="Z82" s="27"/>
     </row>
     <row r="83" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="41" t="s">
+      <c r="A83" s="108" t="s">
         <v>102</v>
       </c>
       <c r="B83" s="26" t="s">
@@ -21741,7 +21743,7 @@
       <c r="Z83" s="27"/>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="41" t="s">
+      <c r="A84" s="108" t="s">
         <v>103</v>
       </c>
       <c r="B84" s="26" t="s">
@@ -21785,7 +21787,7 @@
       <c r="Z84" s="27"/>
     </row>
     <row r="85" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="41" t="s">
+      <c r="A85" s="108" t="s">
         <v>104</v>
       </c>
       <c r="B85" s="26" t="s">
@@ -21865,7 +21867,7 @@
       <c r="Z86" s="48"/>
     </row>
     <row r="87" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="41" t="s">
+      <c r="A87" s="108" t="s">
         <v>108</v>
       </c>
       <c r="B87" s="26" t="s">
@@ -21909,7 +21911,7 @@
       <c r="Z87" s="27"/>
     </row>
     <row r="88" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="41" t="s">
+      <c r="A88" s="108" t="s">
         <v>109</v>
       </c>
       <c r="B88" s="26" t="s">
@@ -21953,7 +21955,7 @@
       <c r="Z88" s="27"/>
     </row>
     <row r="89" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="41" t="s">
+      <c r="A89" s="108" t="s">
         <v>110</v>
       </c>
       <c r="B89" s="26" t="s">
@@ -21997,7 +21999,7 @@
       <c r="Z89" s="27"/>
     </row>
     <row r="90" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="41" t="s">
+      <c r="A90" s="108" t="s">
         <v>111</v>
       </c>
       <c r="B90" s="26" t="s">
@@ -22041,7 +22043,7 @@
       <c r="Z90" s="27"/>
     </row>
     <row r="91" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="41" t="s">
+      <c r="A91" s="108" t="s">
         <v>112</v>
       </c>
       <c r="B91" s="26" t="s">
@@ -22085,7 +22087,7 @@
       <c r="Z91" s="27"/>
     </row>
     <row r="92" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="41" t="s">
+      <c r="A92" s="108" t="s">
         <v>113</v>
       </c>
       <c r="B92" s="26" t="s">
@@ -22129,7 +22131,7 @@
       <c r="Z92" s="27"/>
     </row>
     <row r="93" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="41" t="s">
+      <c r="A93" s="108" t="s">
         <v>114</v>
       </c>
       <c r="B93" s="26" t="s">
@@ -22173,7 +22175,7 @@
       <c r="Z93" s="27"/>
     </row>
     <row r="94" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="41" t="s">
+      <c r="A94" s="108" t="s">
         <v>115</v>
       </c>
       <c r="B94" s="26" t="s">
@@ -22217,7 +22219,7 @@
       <c r="Z94" s="27"/>
     </row>
     <row r="95" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="41" t="s">
+      <c r="A95" s="108" t="s">
         <v>116</v>
       </c>
       <c r="B95" s="26" t="s">
@@ -22261,7 +22263,7 @@
       <c r="Z95" s="27"/>
     </row>
     <row r="96" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="41" t="s">
+      <c r="A96" s="108" t="s">
         <v>117</v>
       </c>
       <c r="B96" s="26" t="s">
@@ -22305,7 +22307,7 @@
       <c r="Z96" s="27"/>
     </row>
     <row r="97" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="41" t="s">
+      <c r="A97" s="108" t="s">
         <v>118</v>
       </c>
       <c r="B97" s="26" t="s">
@@ -22349,7 +22351,7 @@
       <c r="Z97" s="27"/>
     </row>
     <row r="98" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="41" t="s">
+      <c r="A98" s="108" t="s">
         <v>119</v>
       </c>
       <c r="B98" s="26" t="s">
@@ -22393,7 +22395,7 @@
       <c r="Z98" s="27"/>
     </row>
     <row r="99" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="41" t="s">
+      <c r="A99" s="108" t="s">
         <v>120</v>
       </c>
       <c r="B99" s="26" t="s">
@@ -22437,7 +22439,7 @@
       <c r="Z99" s="27"/>
     </row>
     <row r="100" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="41" t="s">
+      <c r="A100" s="108" t="s">
         <v>121</v>
       </c>
       <c r="B100" s="26" t="s">
@@ -22481,7 +22483,7 @@
       <c r="Z100" s="27"/>
     </row>
     <row r="101" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="41" t="s">
+      <c r="A101" s="108" t="s">
         <v>122</v>
       </c>
       <c r="B101" s="26" t="s">
@@ -22525,7 +22527,7 @@
       <c r="Z101" s="27"/>
     </row>
     <row r="102" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="41" t="s">
+      <c r="A102" s="108" t="s">
         <v>123</v>
       </c>
       <c r="B102" s="26" t="s">
@@ -22569,7 +22571,7 @@
       <c r="Z102" s="27"/>
     </row>
     <row r="103" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="41" t="s">
+      <c r="A103" s="108" t="s">
         <v>124</v>
       </c>
       <c r="B103" s="26" t="s">
@@ -22613,7 +22615,7 @@
       <c r="Z103" s="27"/>
     </row>
     <row r="104" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="41" t="s">
+      <c r="A104" s="108" t="s">
         <v>125</v>
       </c>
       <c r="B104" s="26" t="s">
@@ -22657,7 +22659,7 @@
       <c r="Z104" s="27"/>
     </row>
     <row r="105" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="41" t="s">
+      <c r="A105" s="108" t="s">
         <v>126</v>
       </c>
       <c r="B105" s="26" t="s">
@@ -22701,7 +22703,7 @@
       <c r="Z105" s="27"/>
     </row>
     <row r="106" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="41" t="s">
+      <c r="A106" s="108" t="s">
         <v>127</v>
       </c>
       <c r="B106" s="26" t="s">
@@ -22781,7 +22783,7 @@
       <c r="Z107" s="52"/>
     </row>
     <row r="108" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="56" t="s">
+      <c r="A108" s="109" t="s">
         <v>131</v>
       </c>
       <c r="B108" s="26" t="s">
@@ -22825,7 +22827,7 @@
       <c r="Z108" s="27"/>
     </row>
     <row r="109" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="56" t="s">
+      <c r="A109" s="109" t="s">
         <v>132</v>
       </c>
       <c r="B109" s="26" t="s">
@@ -22869,7 +22871,7 @@
       <c r="Z109" s="27"/>
     </row>
     <row r="110" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="56" t="s">
+      <c r="A110" s="109" t="s">
         <v>133</v>
       </c>
       <c r="B110" s="26" t="s">
@@ -22913,7 +22915,7 @@
       <c r="Z110" s="27"/>
     </row>
     <row r="111" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="56" t="s">
+      <c r="A111" s="109" t="s">
         <v>134</v>
       </c>
       <c r="B111" s="26" t="s">
@@ -22957,7 +22959,7 @@
       <c r="Z111" s="27"/>
     </row>
     <row r="112" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="56" t="s">
+      <c r="A112" s="109" t="s">
         <v>135</v>
       </c>
       <c r="B112" s="26" t="s">
@@ -23001,7 +23003,7 @@
       <c r="Z112" s="27"/>
     </row>
     <row r="113" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="56" t="s">
+      <c r="A113" s="109" t="s">
         <v>136</v>
       </c>
       <c r="B113" s="26" t="s">
@@ -23045,7 +23047,7 @@
       <c r="Z113" s="27"/>
     </row>
     <row r="114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="56" t="s">
+      <c r="A114" s="109" t="s">
         <v>137</v>
       </c>
       <c r="B114" s="26" t="s">
@@ -23089,7 +23091,7 @@
       <c r="Z114" s="27"/>
     </row>
     <row r="115" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="56" t="s">
+      <c r="A115" s="109" t="s">
         <v>138</v>
       </c>
       <c r="B115" s="26" t="s">
@@ -23133,7 +23135,7 @@
       <c r="Z115" s="27"/>
     </row>
     <row r="116" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="56" t="s">
+      <c r="A116" s="109" t="s">
         <v>139</v>
       </c>
       <c r="B116" s="26" t="s">
@@ -23177,7 +23179,7 @@
       <c r="Z116" s="27"/>
     </row>
     <row r="117" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="56" t="s">
+      <c r="A117" s="109" t="s">
         <v>140</v>
       </c>
       <c r="B117" s="26" t="s">
@@ -23221,7 +23223,7 @@
       <c r="Z117" s="27"/>
     </row>
     <row r="118" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="56" t="s">
+      <c r="A118" s="109" t="s">
         <v>141</v>
       </c>
       <c r="B118" s="26" t="s">
@@ -23265,7 +23267,7 @@
       <c r="Z118" s="27"/>
     </row>
     <row r="119" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="56" t="s">
+      <c r="A119" s="109" t="s">
         <v>142</v>
       </c>
       <c r="B119" s="26" t="s">
@@ -23309,7 +23311,7 @@
       <c r="Z119" s="27"/>
     </row>
     <row r="120" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="56" t="s">
+      <c r="A120" s="109" t="s">
         <v>143</v>
       </c>
       <c r="B120" s="26" t="s">
@@ -23353,7 +23355,7 @@
       <c r="Z120" s="27"/>
     </row>
     <row r="121" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="56" t="s">
+      <c r="A121" s="109" t="s">
         <v>144</v>
       </c>
       <c r="B121" s="26" t="s">
@@ -23397,7 +23399,7 @@
       <c r="Z121" s="27"/>
     </row>
     <row r="122" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="56" t="s">
+      <c r="A122" s="109" t="s">
         <v>145</v>
       </c>
       <c r="B122" s="26" t="s">
@@ -23441,7 +23443,7 @@
       <c r="Z122" s="27"/>
     </row>
     <row r="123" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="56" t="s">
+      <c r="A123" s="109" t="s">
         <v>146</v>
       </c>
       <c r="B123" s="26" t="s">
@@ -23485,7 +23487,7 @@
       <c r="Z123" s="27"/>
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="56" t="s">
+      <c r="A124" s="109" t="s">
         <v>147</v>
       </c>
       <c r="B124" s="26" t="s">
@@ -23529,7 +23531,7 @@
       <c r="Z124" s="27"/>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="56" t="s">
+      <c r="A125" s="109" t="s">
         <v>148</v>
       </c>
       <c r="B125" s="26" t="s">
@@ -23573,7 +23575,7 @@
       <c r="Z125" s="27"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="56" t="s">
+      <c r="A126" s="109" t="s">
         <v>149</v>
       </c>
       <c r="B126" s="26" t="s">
@@ -23617,7 +23619,7 @@
       <c r="Z126" s="27"/>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="56" t="s">
+      <c r="A127" s="109" t="s">
         <v>150</v>
       </c>
       <c r="B127" s="26" t="s">
@@ -23693,7 +23695,7 @@
       <c r="Z128" s="58"/>
     </row>
     <row r="129" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="56" t="s">
+      <c r="A129" s="109" t="s">
         <v>152</v>
       </c>
       <c r="B129" s="26" t="s">
@@ -23737,7 +23739,7 @@
       <c r="Z129" s="27"/>
     </row>
     <row r="130" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="56" t="s">
+      <c r="A130" s="109" t="s">
         <v>153</v>
       </c>
       <c r="B130" s="26" t="s">
@@ -23781,7 +23783,7 @@
       <c r="Z130" s="27"/>
     </row>
     <row r="131" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="56" t="s">
+      <c r="A131" s="109" t="s">
         <v>154</v>
       </c>
       <c r="B131" s="26" t="s">
@@ -23825,7 +23827,7 @@
       <c r="Z131" s="27"/>
     </row>
     <row r="132" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="56" t="s">
+      <c r="A132" s="109" t="s">
         <v>155</v>
       </c>
       <c r="B132" s="26" t="s">
@@ -23869,7 +23871,7 @@
       <c r="Z132" s="27"/>
     </row>
     <row r="133" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="56" t="s">
+      <c r="A133" s="109" t="s">
         <v>156</v>
       </c>
       <c r="B133" s="26" t="s">
@@ -23913,7 +23915,7 @@
       <c r="Z133" s="27"/>
     </row>
     <row r="134" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="56" t="s">
+      <c r="A134" s="109" t="s">
         <v>157</v>
       </c>
       <c r="B134" s="26" t="s">
@@ -23957,7 +23959,7 @@
       <c r="Z134" s="27"/>
     </row>
     <row r="135" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="56" t="s">
+      <c r="A135" s="109" t="s">
         <v>158</v>
       </c>
       <c r="B135" s="26" t="s">
@@ -24001,7 +24003,7 @@
       <c r="Z135" s="27"/>
     </row>
     <row r="136" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="56" t="s">
+      <c r="A136" s="109" t="s">
         <v>159</v>
       </c>
       <c r="B136" s="26" t="s">
@@ -24045,7 +24047,7 @@
       <c r="Z136" s="27"/>
     </row>
     <row r="137" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="56" t="s">
+      <c r="A137" s="109" t="s">
         <v>160</v>
       </c>
       <c r="B137" s="26" t="s">
@@ -24089,7 +24091,7 @@
       <c r="Z137" s="27"/>
     </row>
     <row r="138" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="56" t="s">
+      <c r="A138" s="109" t="s">
         <v>161</v>
       </c>
       <c r="B138" s="26" t="s">
@@ -24505,7 +24507,7 @@
       <c r="Z147" s="97"/>
     </row>
     <row r="148" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="56" t="s">
+      <c r="A148" s="109" t="s">
         <v>187</v>
       </c>
       <c r="B148" s="26" t="s">
@@ -32444,7 +32446,7 @@
       <c r="H995" s="75"/>
     </row>
     <row r="996" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A996" s="72"/>
+      <c r="A996" s="8"/>
       <c r="B996" s="71"/>
       <c r="C996" s="71"/>
       <c r="D996" s="71"/>
@@ -32459,7 +32461,7 @@
       </c>
     </row>
     <row r="997" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A997" s="72"/>
+      <c r="A997" s="8"/>
       <c r="B997" s="71"/>
       <c r="C997" s="71"/>
       <c r="D997" s="71"/>
@@ -32471,7 +32473,7 @@
       <c r="J997" s="90"/>
     </row>
     <row r="998" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A998" s="72"/>
+      <c r="A998" s="8"/>
       <c r="B998" s="71"/>
       <c r="C998" s="71"/>
       <c r="D998" s="71"/>
@@ -32483,7 +32485,7 @@
       <c r="J998" s="90"/>
     </row>
     <row r="999" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A999" s="72"/>
+      <c r="A999" s="8"/>
       <c r="B999" s="71"/>
       <c r="C999" s="71"/>
       <c r="D999" s="71"/>
@@ -32495,7 +32497,7 @@
       <c r="J999" s="90"/>
     </row>
     <row r="1000" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1000" s="72"/>
+      <c r="A1000" s="8"/>
       <c r="B1000" s="71"/>
       <c r="C1000" s="71"/>
       <c r="D1000" s="71"/>
@@ -32507,7 +32509,7 @@
       <c r="J1000" s="90"/>
     </row>
     <row r="1001" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1001" s="72"/>
+      <c r="A1001" s="8"/>
       <c r="B1001" s="71"/>
       <c r="C1001" s="71"/>
       <c r="D1001" s="71"/>
@@ -32519,7 +32521,7 @@
       <c r="J1001" s="90"/>
     </row>
     <row r="1002" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1002" s="72"/>
+      <c r="A1002" s="8"/>
       <c r="B1002" s="71"/>
       <c r="C1002" s="71"/>
       <c r="D1002" s="71"/>
@@ -32531,7 +32533,7 @@
       <c r="J1002" s="90"/>
     </row>
     <row r="1003" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1003" s="72"/>
+      <c r="A1003" s="8"/>
       <c r="B1003" s="71"/>
       <c r="C1003" s="71"/>
       <c r="D1003" s="71"/>
@@ -32543,7 +32545,7 @@
       <c r="J1003" s="90"/>
     </row>
     <row r="1004" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1004" s="72"/>
+      <c r="A1004" s="8"/>
       <c r="B1004" s="71"/>
       <c r="C1004" s="71"/>
       <c r="D1004" s="71"/>
@@ -32555,7 +32557,7 @@
       <c r="J1004" s="90"/>
     </row>
     <row r="1005" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1005" s="72"/>
+      <c r="A1005" s="8"/>
       <c r="B1005" s="71"/>
       <c r="C1005" s="71"/>
       <c r="D1005" s="71"/>
@@ -32567,7 +32569,7 @@
       <c r="J1005" s="90"/>
     </row>
     <row r="1006" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1006" s="72"/>
+      <c r="A1006" s="8"/>
       <c r="B1006" s="71"/>
       <c r="C1006" s="71"/>
       <c r="D1006" s="71"/>
@@ -32579,7 +32581,7 @@
       <c r="J1006" s="90"/>
     </row>
     <row r="1007" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1007" s="72"/>
+      <c r="A1007" s="8"/>
       <c r="B1007" s="71"/>
       <c r="C1007" s="71"/>
       <c r="D1007" s="71"/>
@@ -32591,7 +32593,7 @@
       <c r="J1007" s="90"/>
     </row>
     <row r="1008" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1008" s="72"/>
+      <c r="A1008" s="8"/>
       <c r="B1008" s="71"/>
       <c r="C1008" s="71"/>
       <c r="D1008" s="71"/>
@@ -32603,7 +32605,7 @@
       <c r="J1008" s="90"/>
     </row>
     <row r="1009" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1009" s="72"/>
+      <c r="A1009" s="8"/>
       <c r="B1009" s="71"/>
       <c r="C1009" s="71"/>
       <c r="D1009" s="71"/>
@@ -32615,7 +32617,7 @@
       <c r="J1009" s="90"/>
     </row>
     <row r="1010" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1010" s="72"/>
+      <c r="A1010" s="8"/>
       <c r="B1010" s="71"/>
       <c r="C1010" s="71"/>
       <c r="D1010" s="71"/>
@@ -32627,7 +32629,7 @@
       <c r="J1010" s="90"/>
     </row>
     <row r="1011" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1011" s="72"/>
+      <c r="A1011" s="8"/>
       <c r="B1011" s="71"/>
       <c r="C1011" s="71"/>
       <c r="D1011" s="71"/>
@@ -32639,7 +32641,7 @@
       <c r="J1011" s="90"/>
     </row>
     <row r="1012" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1012" s="72"/>
+      <c r="A1012" s="8"/>
       <c r="B1012" s="71"/>
       <c r="C1012" s="71"/>
       <c r="D1012" s="71"/>
@@ -32651,7 +32653,7 @@
       <c r="J1012" s="90"/>
     </row>
     <row r="1013" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1013" s="72"/>
+      <c r="A1013" s="8"/>
       <c r="B1013" s="71"/>
       <c r="C1013" s="71"/>
       <c r="D1013" s="71"/>
@@ -32663,7 +32665,7 @@
       <c r="J1013" s="90"/>
     </row>
     <row r="1014" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1014" s="72"/>
+      <c r="A1014" s="8"/>
       <c r="B1014" s="71"/>
       <c r="C1014" s="71"/>
       <c r="D1014" s="71"/>
@@ -32675,7 +32677,7 @@
       <c r="J1014" s="90"/>
     </row>
     <row r="1015" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1015" s="72"/>
+      <c r="A1015" s="8"/>
       <c r="B1015" s="71"/>
       <c r="C1015" s="71"/>
       <c r="D1015" s="71"/>
@@ -32687,7 +32689,7 @@
       <c r="J1015" s="90"/>
     </row>
     <row r="1016" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1016" s="72"/>
+      <c r="A1016" s="8"/>
       <c r="B1016" s="71"/>
       <c r="C1016" s="71"/>
       <c r="D1016" s="71"/>
@@ -32699,7 +32701,7 @@
       <c r="J1016" s="90"/>
     </row>
     <row r="1017" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1017" s="72"/>
+      <c r="A1017" s="8"/>
       <c r="B1017" s="71"/>
       <c r="C1017" s="71"/>
       <c r="D1017" s="71"/>
@@ -32711,7 +32713,7 @@
       <c r="J1017" s="90"/>
     </row>
     <row r="1018" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1018" s="72"/>
+      <c r="A1018" s="8"/>
       <c r="B1018" s="71"/>
       <c r="C1018" s="71"/>
       <c r="D1018" s="71"/>
@@ -32723,7 +32725,7 @@
       <c r="J1018" s="90"/>
     </row>
     <row r="1019" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1019" s="72"/>
+      <c r="A1019" s="8"/>
       <c r="B1019" s="71"/>
       <c r="C1019" s="71"/>
       <c r="D1019" s="71"/>
@@ -32735,7 +32737,7 @@
       <c r="J1019" s="90"/>
     </row>
     <row r="1020" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1020" s="72"/>
+      <c r="A1020" s="8"/>
       <c r="B1020" s="71"/>
       <c r="C1020" s="71"/>
       <c r="D1020" s="71"/>
@@ -32747,7 +32749,7 @@
       <c r="J1020" s="90"/>
     </row>
     <row r="1021" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1021" s="72"/>
+      <c r="A1021" s="8"/>
       <c r="B1021" s="71"/>
       <c r="C1021" s="71"/>
       <c r="D1021" s="71"/>
@@ -32759,7 +32761,7 @@
       <c r="J1021" s="90"/>
     </row>
     <row r="1022" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1022" s="72"/>
+      <c r="A1022" s="8"/>
       <c r="B1022" s="71"/>
       <c r="C1022" s="71"/>
       <c r="D1022" s="71"/>
@@ -32771,7 +32773,7 @@
       <c r="J1022" s="90"/>
     </row>
     <row r="1023" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1023" s="72"/>
+      <c r="A1023" s="8"/>
       <c r="B1023" s="71"/>
       <c r="C1023" s="71"/>
       <c r="D1023" s="71"/>
@@ -32783,7 +32785,7 @@
       <c r="J1023" s="90"/>
     </row>
     <row r="1024" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1024" s="72"/>
+      <c r="A1024" s="8"/>
       <c r="B1024" s="71"/>
       <c r="C1024" s="71"/>
       <c r="D1024" s="71"/>
@@ -32795,7 +32797,7 @@
       <c r="J1024" s="90"/>
     </row>
     <row r="1025" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1025" s="72"/>
+      <c r="A1025" s="8"/>
       <c r="B1025" s="71"/>
       <c r="C1025" s="71"/>
       <c r="D1025" s="71"/>
@@ -32807,7 +32809,7 @@
       <c r="J1025" s="90"/>
     </row>
     <row r="1026" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1026" s="72"/>
+      <c r="A1026" s="8"/>
       <c r="B1026" s="71"/>
       <c r="C1026" s="71"/>
       <c r="D1026" s="71"/>
@@ -32819,7 +32821,7 @@
       <c r="J1026" s="90"/>
     </row>
     <row r="1027" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1027" s="72"/>
+      <c r="A1027" s="8"/>
       <c r="B1027" s="71"/>
       <c r="C1027" s="71"/>
       <c r="D1027" s="71"/>
@@ -32831,7 +32833,7 @@
       <c r="J1027" s="90"/>
     </row>
     <row r="1028" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1028" s="72"/>
+      <c r="A1028" s="8"/>
       <c r="B1028" s="71"/>
       <c r="C1028" s="71"/>
       <c r="D1028" s="71"/>
@@ -32843,7 +32845,7 @@
       <c r="J1028" s="90"/>
     </row>
     <row r="1029" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1029" s="72"/>
+      <c r="A1029" s="8"/>
       <c r="B1029" s="71"/>
       <c r="C1029" s="71"/>
       <c r="D1029" s="71"/>
@@ -32855,7 +32857,7 @@
       <c r="J1029" s="90"/>
     </row>
     <row r="1030" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1030" s="72"/>
+      <c r="A1030" s="8"/>
       <c r="B1030" s="71"/>
       <c r="C1030" s="71"/>
       <c r="D1030" s="71"/>
@@ -32867,7 +32869,7 @@
       <c r="J1030" s="90"/>
     </row>
     <row r="1031" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1031" s="72"/>
+      <c r="A1031" s="8"/>
       <c r="B1031" s="71"/>
       <c r="C1031" s="71"/>
       <c r="D1031" s="71"/>
@@ -32879,7 +32881,7 @@
       <c r="J1031" s="90"/>
     </row>
     <row r="1032" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1032" s="72"/>
+      <c r="A1032" s="8"/>
       <c r="B1032" s="71"/>
       <c r="C1032" s="71"/>
       <c r="D1032" s="71"/>
@@ -32891,7 +32893,7 @@
       <c r="J1032" s="90"/>
     </row>
     <row r="1033" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1033" s="72"/>
+      <c r="A1033" s="8"/>
       <c r="B1033" s="71"/>
       <c r="C1033" s="71"/>
       <c r="D1033" s="71"/>
@@ -32903,7 +32905,7 @@
       <c r="J1033" s="90"/>
     </row>
     <row r="1034" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1034" s="72"/>
+      <c r="A1034" s="8"/>
       <c r="B1034" s="71"/>
       <c r="C1034" s="71"/>
       <c r="D1034" s="71"/>
@@ -32915,7 +32917,7 @@
       <c r="J1034" s="90"/>
     </row>
     <row r="1035" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1035" s="72"/>
+      <c r="A1035" s="8"/>
       <c r="B1035" s="71"/>
       <c r="C1035" s="71"/>
       <c r="D1035" s="71"/>
@@ -32927,7 +32929,7 @@
       <c r="J1035" s="90"/>
     </row>
     <row r="1036" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1036" s="72"/>
+      <c r="A1036" s="8"/>
       <c r="B1036" s="71"/>
       <c r="C1036" s="71"/>
       <c r="D1036" s="71"/>
@@ -32939,7 +32941,7 @@
       <c r="J1036" s="90"/>
     </row>
     <row r="1037" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1037" s="72"/>
+      <c r="A1037" s="8"/>
       <c r="B1037" s="71"/>
       <c r="C1037" s="71"/>
       <c r="D1037" s="71"/>
@@ -32951,7 +32953,7 @@
       <c r="J1037" s="90"/>
     </row>
     <row r="1038" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1038" s="72"/>
+      <c r="A1038" s="8"/>
       <c r="B1038" s="71"/>
       <c r="C1038" s="71"/>
       <c r="D1038" s="71"/>
@@ -32963,7 +32965,7 @@
       <c r="J1038" s="90"/>
     </row>
     <row r="1039" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1039" s="72"/>
+      <c r="A1039" s="8"/>
       <c r="B1039" s="71"/>
       <c r="C1039" s="71"/>
       <c r="D1039" s="71"/>
@@ -32975,7 +32977,7 @@
       <c r="J1039" s="90"/>
     </row>
     <row r="1040" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1040" s="72"/>
+      <c r="A1040" s="8"/>
       <c r="B1040" s="71"/>
       <c r="C1040" s="71"/>
       <c r="D1040" s="71"/>
@@ -32987,7 +32989,7 @@
       <c r="J1040" s="90"/>
     </row>
     <row r="1041" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1041" s="72"/>
+      <c r="A1041" s="8"/>
       <c r="B1041" s="71"/>
       <c r="C1041" s="71"/>
       <c r="D1041" s="71"/>
@@ -32999,7 +33001,7 @@
       <c r="J1041" s="90"/>
     </row>
     <row r="1042" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1042" s="72"/>
+      <c r="A1042" s="8"/>
       <c r="B1042" s="71"/>
       <c r="C1042" s="71"/>
       <c r="D1042" s="71"/>
@@ -33011,7 +33013,7 @@
       <c r="J1042" s="90"/>
     </row>
     <row r="1043" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1043" s="72"/>
+      <c r="A1043" s="8"/>
       <c r="B1043" s="71"/>
       <c r="C1043" s="71"/>
       <c r="D1043" s="71"/>
@@ -33023,7 +33025,7 @@
       <c r="J1043" s="90"/>
     </row>
     <row r="1044" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1044" s="72"/>
+      <c r="A1044" s="8"/>
       <c r="B1044" s="71"/>
       <c r="C1044" s="71"/>
       <c r="D1044" s="71"/>
@@ -33035,7 +33037,7 @@
       <c r="J1044" s="90"/>
     </row>
     <row r="1045" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1045" s="72"/>
+      <c r="A1045" s="8"/>
       <c r="B1045" s="71"/>
       <c r="C1045" s="71"/>
       <c r="D1045" s="71"/>
@@ -33047,7 +33049,7 @@
       <c r="J1045" s="90"/>
     </row>
     <row r="1046" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1046" s="72"/>
+      <c r="A1046" s="8"/>
       <c r="B1046" s="71"/>
       <c r="C1046" s="71"/>
       <c r="D1046" s="71"/>
@@ -33059,7 +33061,7 @@
       <c r="J1046" s="90"/>
     </row>
     <row r="1047" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1047" s="72"/>
+      <c r="A1047" s="8"/>
       <c r="B1047" s="71"/>
       <c r="C1047" s="71"/>
       <c r="D1047" s="71"/>
@@ -33071,7 +33073,7 @@
       <c r="J1047" s="90"/>
     </row>
     <row r="1048" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1048" s="72"/>
+      <c r="A1048" s="8"/>
       <c r="B1048" s="71"/>
       <c r="C1048" s="71"/>
       <c r="D1048" s="71"/>
@@ -33083,7 +33085,7 @@
       <c r="J1048" s="90"/>
     </row>
     <row r="1049" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1049" s="72"/>
+      <c r="A1049" s="8"/>
       <c r="B1049" s="71"/>
       <c r="C1049" s="71"/>
       <c r="D1049" s="71"/>
@@ -33095,7 +33097,7 @@
       <c r="J1049" s="90"/>
     </row>
     <row r="1050" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1050" s="72"/>
+      <c r="A1050" s="8"/>
       <c r="B1050" s="71"/>
       <c r="C1050" s="71"/>
       <c r="D1050" s="71"/>
@@ -33107,7 +33109,7 @@
       <c r="J1050" s="90"/>
     </row>
     <row r="1051" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1051" s="72"/>
+      <c r="A1051" s="8"/>
       <c r="B1051" s="71"/>
       <c r="C1051" s="71"/>
       <c r="D1051" s="71"/>
@@ -33119,7 +33121,7 @@
       <c r="J1051" s="90"/>
     </row>
     <row r="1052" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1052" s="72"/>
+      <c r="A1052" s="8"/>
       <c r="B1052" s="71"/>
       <c r="C1052" s="71"/>
       <c r="D1052" s="71"/>
@@ -33131,7 +33133,7 @@
       <c r="J1052" s="90"/>
     </row>
     <row r="1053" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1053" s="72"/>
+      <c r="A1053" s="8"/>
       <c r="B1053" s="71"/>
       <c r="C1053" s="71"/>
       <c r="D1053" s="71"/>
@@ -33143,7 +33145,7 @@
       <c r="J1053" s="90"/>
     </row>
     <row r="1054" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1054" s="72"/>
+      <c r="A1054" s="8"/>
       <c r="B1054" s="71"/>
       <c r="C1054" s="71"/>
       <c r="D1054" s="71"/>
@@ -33155,7 +33157,7 @@
       <c r="J1054" s="90"/>
     </row>
     <row r="1055" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1055" s="72"/>
+      <c r="A1055" s="8"/>
       <c r="B1055" s="71"/>
       <c r="C1055" s="71"/>
       <c r="D1055" s="71"/>
@@ -33167,7 +33169,7 @@
       <c r="J1055" s="90"/>
     </row>
     <row r="1056" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1056" s="72"/>
+      <c r="A1056" s="8"/>
       <c r="B1056" s="71"/>
       <c r="C1056" s="71"/>
       <c r="D1056" s="71"/>
@@ -33179,7 +33181,7 @@
       <c r="J1056" s="90"/>
     </row>
     <row r="1057" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1057" s="72"/>
+      <c r="A1057" s="8"/>
       <c r="B1057" s="71"/>
       <c r="C1057" s="71"/>
       <c r="D1057" s="71"/>
@@ -33191,7 +33193,7 @@
       <c r="J1057" s="90"/>
     </row>
     <row r="1058" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1058" s="72"/>
+      <c r="A1058" s="8"/>
       <c r="B1058" s="71"/>
       <c r="C1058" s="71"/>
       <c r="D1058" s="71"/>
@@ -33203,7 +33205,7 @@
       <c r="J1058" s="90"/>
     </row>
     <row r="1059" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1059" s="72"/>
+      <c r="A1059" s="8"/>
       <c r="B1059" s="71"/>
       <c r="C1059" s="71"/>
       <c r="D1059" s="71"/>
@@ -33215,7 +33217,7 @@
       <c r="J1059" s="90"/>
     </row>
     <row r="1060" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1060" s="72"/>
+      <c r="A1060" s="8"/>
       <c r="B1060" s="71"/>
       <c r="C1060" s="71"/>
       <c r="D1060" s="71"/>
@@ -33227,7 +33229,7 @@
       <c r="J1060" s="90"/>
     </row>
     <row r="1061" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1061" s="72"/>
+      <c r="A1061" s="8"/>
       <c r="B1061" s="71"/>
       <c r="C1061" s="71"/>
       <c r="D1061" s="71"/>
@@ -33239,7 +33241,7 @@
       <c r="J1061" s="90"/>
     </row>
     <row r="1062" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1062" s="72"/>
+      <c r="A1062" s="8"/>
       <c r="B1062" s="71"/>
       <c r="C1062" s="71"/>
       <c r="D1062" s="71"/>
@@ -33251,7 +33253,7 @@
       <c r="J1062" s="90"/>
     </row>
     <row r="1063" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1063" s="72"/>
+      <c r="A1063" s="8"/>
       <c r="B1063" s="71"/>
       <c r="C1063" s="71"/>
       <c r="D1063" s="71"/>
@@ -33263,7 +33265,7 @@
       <c r="J1063" s="90"/>
     </row>
     <row r="1064" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1064" s="72"/>
+      <c r="A1064" s="8"/>
       <c r="B1064" s="71"/>
       <c r="C1064" s="71"/>
       <c r="D1064" s="71"/>
@@ -33275,7 +33277,7 @@
       <c r="J1064" s="90"/>
     </row>
     <row r="1065" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1065" s="72"/>
+      <c r="A1065" s="8"/>
       <c r="B1065" s="71"/>
       <c r="C1065" s="71"/>
       <c r="D1065" s="71"/>
@@ -33287,7 +33289,7 @@
       <c r="J1065" s="90"/>
     </row>
     <row r="1066" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1066" s="72"/>
+      <c r="A1066" s="8"/>
       <c r="B1066" s="71"/>
       <c r="C1066" s="71"/>
       <c r="D1066" s="71"/>
@@ -33299,7 +33301,7 @@
       <c r="J1066" s="90"/>
     </row>
     <row r="1067" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1067" s="72"/>
+      <c r="A1067" s="8"/>
       <c r="B1067" s="71"/>
       <c r="C1067" s="71"/>
       <c r="D1067" s="71"/>
@@ -33311,7 +33313,7 @@
       <c r="J1067" s="90"/>
     </row>
     <row r="1068" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1068" s="72"/>
+      <c r="A1068" s="8"/>
       <c r="B1068" s="71"/>
       <c r="C1068" s="71"/>
       <c r="D1068" s="71"/>
@@ -33323,7 +33325,7 @@
       <c r="J1068" s="90"/>
     </row>
     <row r="1069" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1069" s="72"/>
+      <c r="A1069" s="8"/>
       <c r="B1069" s="71"/>
       <c r="C1069" s="71"/>
       <c r="D1069" s="71"/>
@@ -33335,7 +33337,7 @@
       <c r="J1069" s="90"/>
     </row>
     <row r="1070" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1070" s="72"/>
+      <c r="A1070" s="8"/>
       <c r="B1070" s="71"/>
       <c r="C1070" s="71"/>
       <c r="D1070" s="71"/>
@@ -33347,7 +33349,7 @@
       <c r="J1070" s="90"/>
     </row>
     <row r="1071" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1071" s="72"/>
+      <c r="A1071" s="8"/>
       <c r="B1071" s="71"/>
       <c r="C1071" s="71"/>
       <c r="D1071" s="71"/>
@@ -33359,7 +33361,7 @@
       <c r="J1071" s="90"/>
     </row>
     <row r="1072" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1072" s="72"/>
+      <c r="A1072" s="8"/>
       <c r="B1072" s="71"/>
       <c r="C1072" s="71"/>
       <c r="D1072" s="71"/>
@@ -33371,7 +33373,7 @@
       <c r="J1072" s="90"/>
     </row>
     <row r="1073" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1073" s="72"/>
+      <c r="A1073" s="8"/>
       <c r="B1073" s="71"/>
       <c r="C1073" s="71"/>
       <c r="D1073" s="71"/>
@@ -33383,7 +33385,7 @@
       <c r="J1073" s="90"/>
     </row>
     <row r="1074" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1074" s="72"/>
+      <c r="A1074" s="8"/>
       <c r="B1074" s="71"/>
       <c r="C1074" s="71"/>
       <c r="D1074" s="71"/>
@@ -33395,7 +33397,7 @@
       <c r="J1074" s="90"/>
     </row>
     <row r="1075" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1075" s="72"/>
+      <c r="A1075" s="8"/>
       <c r="B1075" s="71"/>
       <c r="C1075" s="71"/>
       <c r="D1075" s="71"/>
@@ -33407,7 +33409,7 @@
       <c r="J1075" s="90"/>
     </row>
     <row r="1076" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1076" s="72"/>
+      <c r="A1076" s="8"/>
       <c r="B1076" s="71"/>
       <c r="C1076" s="71"/>
       <c r="D1076" s="71"/>
@@ -33419,7 +33421,7 @@
       <c r="J1076" s="90"/>
     </row>
     <row r="1077" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1077" s="72"/>
+      <c r="A1077" s="8"/>
       <c r="B1077" s="71"/>
       <c r="C1077" s="71"/>
       <c r="D1077" s="71"/>
@@ -33431,7 +33433,7 @@
       <c r="J1077" s="90"/>
     </row>
     <row r="1078" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1078" s="72"/>
+      <c r="A1078" s="8"/>
       <c r="B1078" s="71"/>
       <c r="C1078" s="71"/>
       <c r="D1078" s="71"/>
@@ -33443,7 +33445,7 @@
       <c r="J1078" s="90"/>
     </row>
     <row r="1079" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1079" s="72"/>
+      <c r="A1079" s="8"/>
       <c r="B1079" s="71"/>
       <c r="C1079" s="71"/>
       <c r="D1079" s="71"/>
@@ -33455,7 +33457,7 @@
       <c r="J1079" s="90"/>
     </row>
     <row r="1080" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1080" s="72"/>
+      <c r="A1080" s="8"/>
       <c r="B1080" s="71"/>
       <c r="C1080" s="71"/>
       <c r="D1080" s="71"/>
@@ -33467,7 +33469,7 @@
       <c r="J1080" s="90"/>
     </row>
     <row r="1081" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1081" s="72"/>
+      <c r="A1081" s="8"/>
       <c r="B1081" s="71"/>
       <c r="C1081" s="71"/>
       <c r="D1081" s="71"/>
@@ -33479,7 +33481,7 @@
       <c r="J1081" s="90"/>
     </row>
     <row r="1082" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1082" s="72"/>
+      <c r="A1082" s="8"/>
       <c r="B1082" s="71"/>
       <c r="C1082" s="71"/>
       <c r="D1082" s="71"/>
@@ -33491,7 +33493,7 @@
       <c r="J1082" s="90"/>
     </row>
     <row r="1083" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1083" s="72"/>
+      <c r="A1083" s="8"/>
       <c r="B1083" s="71"/>
       <c r="C1083" s="71"/>
       <c r="D1083" s="71"/>
@@ -33503,7 +33505,7 @@
       <c r="J1083" s="90"/>
     </row>
     <row r="1084" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1084" s="72"/>
+      <c r="A1084" s="8"/>
       <c r="B1084" s="71"/>
       <c r="C1084" s="71"/>
       <c r="D1084" s="71"/>
@@ -33515,7 +33517,7 @@
       <c r="J1084" s="90"/>
     </row>
     <row r="1085" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1085" s="72"/>
+      <c r="A1085" s="8"/>
       <c r="B1085" s="71"/>
       <c r="C1085" s="71"/>
       <c r="D1085" s="71"/>
@@ -33527,7 +33529,7 @@
       <c r="J1085" s="90"/>
     </row>
     <row r="1086" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1086" s="72"/>
+      <c r="A1086" s="8"/>
       <c r="B1086" s="71"/>
       <c r="C1086" s="71"/>
       <c r="D1086" s="71"/>
@@ -33539,7 +33541,7 @@
       <c r="J1086" s="90"/>
     </row>
     <row r="1087" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1087" s="72"/>
+      <c r="A1087" s="8"/>
       <c r="B1087" s="71"/>
       <c r="C1087" s="71"/>
       <c r="D1087" s="71"/>
@@ -33551,7 +33553,7 @@
       <c r="J1087" s="90"/>
     </row>
     <row r="1088" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1088" s="72"/>
+      <c r="A1088" s="8"/>
       <c r="B1088" s="71"/>
       <c r="C1088" s="71"/>
       <c r="D1088" s="71"/>
@@ -33563,7 +33565,7 @@
       <c r="J1088" s="90"/>
     </row>
     <row r="1089" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1089" s="72"/>
+      <c r="A1089" s="8"/>
       <c r="B1089" s="71"/>
       <c r="C1089" s="71"/>
       <c r="D1089" s="71"/>
@@ -33575,7 +33577,7 @@
       <c r="J1089" s="90"/>
     </row>
     <row r="1090" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1090" s="72"/>
+      <c r="A1090" s="8"/>
       <c r="B1090" s="71"/>
       <c r="C1090" s="71"/>
       <c r="D1090" s="71"/>
@@ -33587,7 +33589,7 @@
       <c r="J1090" s="90"/>
     </row>
     <row r="1091" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1091" s="72"/>
+      <c r="A1091" s="8"/>
       <c r="B1091" s="71"/>
       <c r="C1091" s="71"/>
       <c r="D1091" s="71"/>
@@ -33599,7 +33601,7 @@
       <c r="J1091" s="90"/>
     </row>
     <row r="1092" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1092" s="72"/>
+      <c r="A1092" s="8"/>
       <c r="B1092" s="71"/>
       <c r="C1092" s="71"/>
       <c r="D1092" s="71"/>
@@ -33611,7 +33613,7 @@
       <c r="J1092" s="90"/>
     </row>
     <row r="1093" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1093" s="72"/>
+      <c r="A1093" s="8"/>
       <c r="B1093" s="71"/>
       <c r="C1093" s="71"/>
       <c r="D1093" s="71"/>
@@ -33623,7 +33625,7 @@
       <c r="J1093" s="90"/>
     </row>
     <row r="1094" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1094" s="72"/>
+      <c r="A1094" s="8"/>
       <c r="B1094" s="71"/>
       <c r="C1094" s="71"/>
       <c r="D1094" s="71"/>
@@ -33635,7 +33637,7 @@
       <c r="J1094" s="90"/>
     </row>
     <row r="1095" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1095" s="72"/>
+      <c r="A1095" s="8"/>
       <c r="B1095" s="71"/>
       <c r="C1095" s="71"/>
       <c r="D1095" s="71"/>
@@ -33647,7 +33649,7 @@
       <c r="J1095" s="90"/>
     </row>
     <row r="1096" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1096" s="72"/>
+      <c r="A1096" s="8"/>
       <c r="B1096" s="71"/>
       <c r="C1096" s="71"/>
       <c r="D1096" s="71"/>
@@ -33659,7 +33661,7 @@
       <c r="J1096" s="90"/>
     </row>
     <row r="1097" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1097" s="72"/>
+      <c r="A1097" s="8"/>
       <c r="B1097" s="71"/>
       <c r="C1097" s="71"/>
       <c r="D1097" s="71"/>
@@ -33671,7 +33673,7 @@
       <c r="J1097" s="90"/>
     </row>
     <row r="1098" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1098" s="72"/>
+      <c r="A1098" s="8"/>
       <c r="B1098" s="71"/>
       <c r="C1098" s="71"/>
       <c r="D1098" s="71"/>
@@ -33683,7 +33685,7 @@
       <c r="J1098" s="90"/>
     </row>
     <row r="1099" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1099" s="72"/>
+      <c r="A1099" s="8"/>
       <c r="B1099" s="71"/>
       <c r="C1099" s="71"/>
       <c r="D1099" s="71"/>
@@ -33695,7 +33697,7 @@
       <c r="J1099" s="90"/>
     </row>
     <row r="1100" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1100" s="72"/>
+      <c r="A1100" s="8"/>
       <c r="B1100" s="71"/>
       <c r="C1100" s="71"/>
       <c r="D1100" s="71"/>
@@ -33707,7 +33709,7 @@
       <c r="J1100" s="90"/>
     </row>
     <row r="1101" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1101" s="72"/>
+      <c r="A1101" s="8"/>
       <c r="B1101" s="71"/>
       <c r="C1101" s="71"/>
       <c r="D1101" s="71"/>
@@ -33719,7 +33721,7 @@
       <c r="J1101" s="90"/>
     </row>
     <row r="1102" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1102" s="72"/>
+      <c r="A1102" s="8"/>
       <c r="B1102" s="71"/>
       <c r="C1102" s="71"/>
       <c r="D1102" s="71"/>
@@ -33731,7 +33733,7 @@
       <c r="J1102" s="90"/>
     </row>
     <row r="1103" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1103" s="72"/>
+      <c r="A1103" s="8"/>
       <c r="B1103" s="71"/>
       <c r="C1103" s="71"/>
       <c r="D1103" s="71"/>
@@ -33743,7 +33745,7 @@
       <c r="J1103" s="90"/>
     </row>
     <row r="1104" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1104" s="72"/>
+      <c r="A1104" s="8"/>
       <c r="B1104" s="71"/>
       <c r="C1104" s="71"/>
       <c r="D1104" s="71"/>
@@ -33755,7 +33757,7 @@
       <c r="J1104" s="90"/>
     </row>
     <row r="1105" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1105" s="72"/>
+      <c r="A1105" s="8"/>
       <c r="B1105" s="71"/>
       <c r="C1105" s="71"/>
       <c r="D1105" s="71"/>
@@ -33767,7 +33769,7 @@
       <c r="J1105" s="90"/>
     </row>
     <row r="1106" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1106" s="72"/>
+      <c r="A1106" s="8"/>
       <c r="B1106" s="71"/>
       <c r="C1106" s="71"/>
       <c r="D1106" s="71"/>
@@ -33779,7 +33781,7 @@
       <c r="J1106" s="90"/>
     </row>
     <row r="1107" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1107" s="72"/>
+      <c r="A1107" s="8"/>
       <c r="B1107" s="71"/>
       <c r="C1107" s="71"/>
       <c r="D1107" s="71"/>
@@ -33791,7 +33793,7 @@
       <c r="J1107" s="90"/>
     </row>
     <row r="1108" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1108" s="72"/>
+      <c r="A1108" s="8"/>
       <c r="B1108" s="71"/>
       <c r="C1108" s="71"/>
       <c r="D1108" s="71"/>
@@ -33803,7 +33805,7 @@
       <c r="J1108" s="90"/>
     </row>
     <row r="1109" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1109" s="72"/>
+      <c r="A1109" s="8"/>
       <c r="B1109" s="71"/>
       <c r="C1109" s="71"/>
       <c r="D1109" s="71"/>
@@ -33815,7 +33817,7 @@
       <c r="J1109" s="90"/>
     </row>
     <row r="1110" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1110" s="72"/>
+      <c r="A1110" s="8"/>
       <c r="B1110" s="71"/>
       <c r="C1110" s="71"/>
       <c r="D1110" s="71"/>
@@ -33827,7 +33829,7 @@
       <c r="J1110" s="90"/>
     </row>
     <row r="1111" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1111" s="72"/>
+      <c r="A1111" s="8"/>
       <c r="B1111" s="71"/>
       <c r="C1111" s="71"/>
       <c r="D1111" s="71"/>
@@ -33839,7 +33841,7 @@
       <c r="J1111" s="90"/>
     </row>
     <row r="1112" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1112" s="72"/>
+      <c r="A1112" s="8"/>
       <c r="B1112" s="71"/>
       <c r="C1112" s="71"/>
       <c r="D1112" s="71"/>
@@ -33851,7 +33853,7 @@
       <c r="J1112" s="90"/>
     </row>
     <row r="1113" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1113" s="72"/>
+      <c r="A1113" s="8"/>
       <c r="B1113" s="71"/>
       <c r="C1113" s="71"/>
       <c r="D1113" s="71"/>
@@ -33863,7 +33865,7 @@
       <c r="J1113" s="90"/>
     </row>
     <row r="1114" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1114" s="72"/>
+      <c r="A1114" s="8"/>
       <c r="B1114" s="71"/>
       <c r="C1114" s="71"/>
       <c r="D1114" s="71"/>
@@ -33875,7 +33877,7 @@
       <c r="J1114" s="90"/>
     </row>
     <row r="1115" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1115" s="72"/>
+      <c r="A1115" s="8"/>
       <c r="B1115" s="71"/>
       <c r="C1115" s="71"/>
       <c r="D1115" s="71"/>
@@ -33903,7 +33905,7 @@
       <c r="Z1115" s="27"/>
     </row>
     <row r="1116" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1116" s="72"/>
+      <c r="A1116" s="8"/>
       <c r="B1116" s="71"/>
       <c r="C1116" s="71"/>
       <c r="D1116" s="71"/>
@@ -33915,7 +33917,7 @@
       <c r="J1116" s="90"/>
     </row>
     <row r="1117" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1117" s="72"/>
+      <c r="A1117" s="8"/>
       <c r="B1117" s="71"/>
       <c r="C1117" s="71"/>
       <c r="D1117" s="71"/>
@@ -33927,7 +33929,7 @@
       <c r="J1117" s="90"/>
     </row>
     <row r="1118" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1118" s="72"/>
+      <c r="A1118" s="8"/>
       <c r="B1118" s="71"/>
       <c r="C1118" s="71"/>
       <c r="D1118" s="71"/>
@@ -33939,7 +33941,7 @@
       <c r="J1118" s="90"/>
     </row>
     <row r="1119" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1119" s="72"/>
+      <c r="A1119" s="8"/>
       <c r="B1119" s="71"/>
       <c r="C1119" s="71"/>
       <c r="D1119" s="71"/>
@@ -33951,7 +33953,7 @@
       <c r="J1119" s="90"/>
     </row>
     <row r="1120" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1120" s="72"/>
+      <c r="A1120" s="8"/>
       <c r="B1120" s="71"/>
       <c r="C1120" s="71"/>
       <c r="D1120" s="71"/>
@@ -33963,7 +33965,7 @@
       <c r="J1120" s="90"/>
     </row>
     <row r="1121" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1121" s="72"/>
+      <c r="A1121" s="8"/>
       <c r="B1121" s="71"/>
       <c r="C1121" s="71"/>
       <c r="D1121" s="71"/>
@@ -33975,7 +33977,7 @@
       <c r="J1121" s="90"/>
     </row>
     <row r="1122" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1122" s="72"/>
+      <c r="A1122" s="8"/>
       <c r="B1122" s="71"/>
       <c r="C1122" s="71"/>
       <c r="D1122" s="71"/>
@@ -33987,7 +33989,7 @@
       <c r="J1122" s="90"/>
     </row>
     <row r="1123" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1123" s="72"/>
+      <c r="A1123" s="8"/>
       <c r="B1123" s="71"/>
       <c r="C1123" s="71"/>
       <c r="D1123" s="71"/>
@@ -33999,7 +34001,7 @@
       <c r="J1123" s="90"/>
     </row>
     <row r="1124" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1124" s="72"/>
+      <c r="A1124" s="8"/>
       <c r="B1124" s="71"/>
       <c r="C1124" s="71"/>
       <c r="D1124" s="71"/>
@@ -34011,7 +34013,7 @@
       <c r="J1124" s="90"/>
     </row>
     <row r="1125" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1125" s="72"/>
+      <c r="A1125" s="8"/>
       <c r="B1125" s="71"/>
       <c r="C1125" s="71"/>
       <c r="D1125" s="71"/>
@@ -34023,7 +34025,7 @@
       <c r="J1125" s="90"/>
     </row>
     <row r="1126" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1126" s="72"/>
+      <c r="A1126" s="8"/>
       <c r="B1126" s="71"/>
       <c r="C1126" s="71"/>
       <c r="D1126" s="71"/>
@@ -34035,7 +34037,7 @@
       <c r="J1126" s="90"/>
     </row>
     <row r="1127" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1127" s="72"/>
+      <c r="A1127" s="8"/>
       <c r="B1127" s="71"/>
       <c r="C1127" s="71"/>
       <c r="D1127" s="71"/>
@@ -34047,7 +34049,7 @@
       <c r="J1127" s="90"/>
     </row>
     <row r="1128" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1128" s="72"/>
+      <c r="A1128" s="8"/>
       <c r="B1128" s="71"/>
       <c r="C1128" s="71"/>
       <c r="D1128" s="71"/>
@@ -34059,7 +34061,7 @@
       <c r="J1128" s="90"/>
     </row>
     <row r="1129" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1129" s="72"/>
+      <c r="A1129" s="8"/>
       <c r="B1129" s="71"/>
       <c r="C1129" s="71"/>
       <c r="D1129" s="71"/>
@@ -34071,7 +34073,7 @@
       <c r="J1129" s="90"/>
     </row>
     <row r="1130" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1130" s="72"/>
+      <c r="A1130" s="8"/>
       <c r="B1130" s="71"/>
       <c r="C1130" s="71"/>
       <c r="D1130" s="71"/>
@@ -34083,7 +34085,7 @@
       <c r="J1130" s="90"/>
     </row>
     <row r="1131" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1131" s="72"/>
+      <c r="A1131" s="8"/>
       <c r="B1131" s="71"/>
       <c r="C1131" s="71"/>
       <c r="D1131" s="71"/>
@@ -34095,7 +34097,7 @@
       <c r="J1131" s="90"/>
     </row>
     <row r="1132" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1132" s="72"/>
+      <c r="A1132" s="8"/>
       <c r="B1132" s="71"/>
       <c r="C1132" s="71"/>
       <c r="D1132" s="71"/>
@@ -34107,7 +34109,7 @@
       <c r="J1132" s="90"/>
     </row>
     <row r="1133" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1133" s="72"/>
+      <c r="A1133" s="8"/>
       <c r="B1133" s="71"/>
       <c r="C1133" s="71"/>
       <c r="D1133" s="71"/>
@@ -34119,7 +34121,7 @@
       <c r="J1133" s="90"/>
     </row>
     <row r="1134" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1134" s="72"/>
+      <c r="A1134" s="8"/>
       <c r="B1134" s="71"/>
       <c r="C1134" s="71"/>
       <c r="D1134" s="71"/>
@@ -34131,7 +34133,7 @@
       <c r="J1134" s="90"/>
     </row>
     <row r="1135" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1135" s="72"/>
+      <c r="A1135" s="8"/>
       <c r="B1135" s="71"/>
       <c r="C1135" s="71"/>
       <c r="D1135" s="71"/>
@@ -34143,7 +34145,7 @@
       <c r="J1135" s="90"/>
     </row>
     <row r="1136" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1136" s="72"/>
+      <c r="A1136" s="8"/>
       <c r="B1136" s="71"/>
       <c r="C1136" s="71"/>
       <c r="D1136" s="71"/>
@@ -34155,7 +34157,7 @@
       <c r="J1136" s="90"/>
     </row>
     <row r="1137" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1137" s="72"/>
+      <c r="A1137" s="8"/>
       <c r="B1137" s="71"/>
       <c r="C1137" s="71"/>
       <c r="D1137" s="71"/>
@@ -34167,7 +34169,7 @@
       <c r="J1137" s="90"/>
     </row>
     <row r="1138" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1138" s="72"/>
+      <c r="A1138" s="8"/>
       <c r="B1138" s="71"/>
       <c r="C1138" s="71"/>
       <c r="D1138" s="71"/>
@@ -34179,7 +34181,7 @@
       <c r="J1138" s="90"/>
     </row>
     <row r="1139" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1139" s="72"/>
+      <c r="A1139" s="8"/>
       <c r="B1139" s="71"/>
       <c r="C1139" s="71"/>
       <c r="D1139" s="71"/>
@@ -34191,7 +34193,7 @@
       <c r="J1139" s="90"/>
     </row>
     <row r="1140" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1140" s="72"/>
+      <c r="A1140" s="8"/>
       <c r="B1140" s="71"/>
       <c r="C1140" s="71"/>
       <c r="D1140" s="71"/>
@@ -34203,7 +34205,7 @@
       <c r="J1140" s="90"/>
     </row>
     <row r="1141" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1141" s="72"/>
+      <c r="A1141" s="8"/>
       <c r="B1141" s="71"/>
       <c r="C1141" s="71"/>
       <c r="D1141" s="71"/>
@@ -34215,7 +34217,7 @@
       <c r="J1141" s="90"/>
     </row>
     <row r="1142" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1142" s="72"/>
+      <c r="A1142" s="8"/>
       <c r="B1142" s="71"/>
       <c r="C1142" s="71"/>
       <c r="D1142" s="71"/>
@@ -34227,7 +34229,7 @@
       <c r="J1142" s="90"/>
     </row>
     <row r="1143" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1143" s="72"/>
+      <c r="A1143" s="8"/>
       <c r="B1143" s="71"/>
       <c r="C1143" s="71"/>
       <c r="D1143" s="71"/>
@@ -34239,7 +34241,7 @@
       <c r="J1143" s="90"/>
     </row>
     <row r="1144" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1144" s="72"/>
+      <c r="A1144" s="8"/>
       <c r="B1144" s="71"/>
       <c r="C1144" s="71"/>
       <c r="D1144" s="71"/>
@@ -34251,7 +34253,7 @@
       <c r="J1144" s="90"/>
     </row>
     <row r="1145" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1145" s="72"/>
+      <c r="A1145" s="8"/>
       <c r="B1145" s="71"/>
       <c r="C1145" s="71"/>
       <c r="D1145" s="71"/>
@@ -34263,7 +34265,7 @@
       <c r="J1145" s="90"/>
     </row>
     <row r="1146" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1146" s="72"/>
+      <c r="A1146" s="8"/>
       <c r="B1146" s="71"/>
       <c r="C1146" s="71"/>
       <c r="D1146" s="71"/>
@@ -34275,7 +34277,7 @@
       <c r="J1146" s="90"/>
     </row>
     <row r="1147" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1147" s="72"/>
+      <c r="A1147" s="8"/>
       <c r="B1147" s="71"/>
       <c r="C1147" s="71"/>
       <c r="D1147" s="71"/>
@@ -34287,7 +34289,7 @@
       <c r="J1147" s="90"/>
     </row>
     <row r="1148" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1148" s="72"/>
+      <c r="A1148" s="8"/>
       <c r="B1148" s="71"/>
       <c r="C1148" s="71"/>
       <c r="D1148" s="71"/>
@@ -34299,7 +34301,7 @@
       <c r="J1148" s="90"/>
     </row>
     <row r="1149" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1149" s="72"/>
+      <c r="A1149" s="8"/>
       <c r="B1149" s="71"/>
       <c r="C1149" s="71"/>
       <c r="D1149" s="71"/>
@@ -34311,7 +34313,7 @@
       <c r="J1149" s="90"/>
     </row>
     <row r="1150" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1150" s="72"/>
+      <c r="A1150" s="8"/>
       <c r="B1150" s="71"/>
       <c r="C1150" s="71"/>
       <c r="D1150" s="71"/>
@@ -34323,7 +34325,7 @@
       <c r="J1150" s="90"/>
     </row>
     <row r="1151" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1151" s="72"/>
+      <c r="A1151" s="8"/>
       <c r="B1151" s="71"/>
       <c r="C1151" s="71"/>
       <c r="D1151" s="71"/>
@@ -34335,7 +34337,7 @@
       <c r="J1151" s="90"/>
     </row>
     <row r="1152" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1152" s="72"/>
+      <c r="A1152" s="8"/>
       <c r="B1152" s="71"/>
       <c r="C1152" s="71"/>
       <c r="D1152" s="71"/>
@@ -34347,7 +34349,7 @@
       <c r="J1152" s="90"/>
     </row>
     <row r="1153" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1153" s="72"/>
+      <c r="A1153" s="8"/>
       <c r="B1153" s="71"/>
       <c r="C1153" s="71"/>
       <c r="D1153" s="71"/>
@@ -34359,7 +34361,7 @@
       <c r="J1153" s="90"/>
     </row>
     <row r="1154" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1154" s="72"/>
+      <c r="A1154" s="8"/>
       <c r="B1154" s="71"/>
       <c r="C1154" s="71"/>
       <c r="D1154" s="71"/>
@@ -34371,7 +34373,7 @@
       <c r="J1154" s="90"/>
     </row>
     <row r="1155" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1155" s="72"/>
+      <c r="A1155" s="8"/>
       <c r="B1155" s="71"/>
       <c r="C1155" s="71"/>
       <c r="D1155" s="71"/>
@@ -34383,7 +34385,7 @@
       <c r="J1155" s="90"/>
     </row>
     <row r="1156" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1156" s="72"/>
+      <c r="A1156" s="8"/>
       <c r="B1156" s="71"/>
       <c r="C1156" s="71"/>
       <c r="D1156" s="71"/>
@@ -34395,7 +34397,7 @@
       <c r="J1156" s="90"/>
     </row>
     <row r="1157" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1157" s="72"/>
+      <c r="A1157" s="8"/>
       <c r="B1157" s="71"/>
       <c r="C1157" s="71"/>
       <c r="D1157" s="71"/>

</xml_diff>

<commit_message>
Now prints out Groups and keywords!
</commit_message>
<xml_diff>
--- a/TestSheet.xlsx
+++ b/TestSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="94" documentId="11_09CE59F3B32C71B27447F41703FFAE311A56176B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BBB6532C-CB74-410F-B275-4D55BA31A760}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="11_09CE59F3B32C71B27447F41703FFAE311A56176B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{173CEE07-C084-43F6-9E27-29C9F8D900B9}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1035" yWindow="1470" windowWidth="18210" windowHeight="10965" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pack Template" sheetId="11" state="hidden" r:id="rId1"/>
@@ -18112,7 +18112,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18178,7 +18178,7 @@
       <c r="G2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="I2" s="20"/>

</xml_diff>